<commit_message>
Add some methods to steel.py, add steel grade data into steel data.
</commit_message>
<xml_diff>
--- a/data/steel_data.xlsx
+++ b/data/steel_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E58651-FBF1-46A6-A9AC-4141F85E9D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D39C5A-149F-463E-82AC-CDDD4337E87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
+    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
   </bookViews>
   <sheets>
     <sheet name="Is" sheetId="1" r:id="rId1"/>
     <sheet name="Cs" sheetId="2" r:id="rId2"/>
+    <sheet name="grades" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="161">
   <si>
     <t>d</t>
   </si>
@@ -467,13 +468,64 @@
   </si>
   <si>
     <t>z_yr</t>
+  </si>
+  <si>
+    <t>f_y</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>f_u</t>
+  </si>
+  <si>
+    <t>C250</t>
+  </si>
+  <si>
+    <t>C350</t>
+  </si>
+  <si>
+    <t>C450</t>
+  </si>
+  <si>
+    <t>AS/NZS1163</t>
+  </si>
+  <si>
+    <t>AS/NZS3678</t>
+  </si>
+  <si>
+    <t>AS/NZS3679.1</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>hollow</t>
+  </si>
+  <si>
+    <t>plate</t>
+  </si>
+  <si>
+    <t>flat and section</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="0.0&quot; kg / m&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00&quot; kg / m&quot;"/>
     <numFmt numFmtId="166" formatCode="0.000&quot; m&quot;"/>
@@ -481,6 +533,7 @@
     <numFmt numFmtId="168" formatCode="##0.00E+00&quot; m⁴&quot;"/>
     <numFmt numFmtId="169" formatCode="##0.00E+00&quot; m³&quot;"/>
     <numFmt numFmtId="170" formatCode="##0.00E+00&quot; m⁶&quot;"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -529,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -540,11 +593,22 @@
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="55">
+    <dxf>
+      <numFmt numFmtId="172" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1815,9 +1879,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="3" xr9:uid="{8A27988E-247C-4FF5-8CF3-24D483E6BCB9}">
-      <tableStyleElement type="wholeTable" dxfId="51"/>
-      <tableStyleElement type="headerRow" dxfId="50"/>
-      <tableStyleElement type="secondRowStripe" dxfId="49"/>
+      <tableStyleElement type="wholeTable" dxfId="54"/>
+      <tableStyleElement type="headerRow" dxfId="53"/>
+      <tableStyleElement type="secondRowStripe" dxfId="52"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1838,65 +1902,81 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:W100" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:W100" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A1:W100" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_type" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="38"/>
-    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="35">
+    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_type" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="41"/>
+    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="38">
       <calculatedColumnFormula>IF(Table2[[#This Row],[w_1]]="",Table2[[#This Row],[r_1]],Table2[[#This Row],[w_1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="34"/>
-    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="33"/>
-    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="32"/>
-    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="31"/>
-    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="30"/>
-    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="29"/>
-    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="28"/>
-    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="27"/>
-    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="26"/>
-    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="25"/>
-    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="37"/>
+    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="36"/>
+    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="35"/>
+    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="34"/>
+    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="33"/>
+    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="32"/>
+    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="31"/>
+    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="30"/>
+    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="29"/>
+    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="28"/>
+    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:V11" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:V11" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:V11" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_type" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="12"/>
-    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="11"/>
-    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="10"/>
-    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="9"/>
-    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="8"/>
-    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="7"/>
-    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="6"/>
-    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="5"/>
-    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="4"/>
-    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="3"/>
-    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="2"/>
-    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="1"/>
-    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_type" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="15"/>
+    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="14"/>
+    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="13"/>
+    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="12"/>
+    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="11"/>
+    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="10"/>
+    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="9"/>
+    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="8"/>
+    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="7"/>
+    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="6"/>
+    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="5"/>
+    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="4"/>
+    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0B154D11-09EB-4C87-921D-9FAEB2520622}" name="Table3" displayName="Table3" ref="A1:G63" totalsRowShown="0">
+  <autoFilter ref="A1:G63" xr:uid="{0B154D11-09EB-4C87-921D-9FAEB2520622}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F624C6BE-779F-496C-A6A5-C90E3B909046}" name="standard"/>
+    <tableColumn id="7" xr3:uid="{F4DBA019-F123-4B98-A615-C1C293EAF7F6}" name="current"/>
+    <tableColumn id="6" xr3:uid="{49F22BD6-5E2F-4DCD-B8F2-753E49B729CD}" name="form"/>
+    <tableColumn id="2" xr3:uid="{D21D031E-2102-48DD-8FDF-9B85CD1F2DC4}" name="grade"/>
+    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2201,7 +2281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DE0702-9028-4C23-A846-1BC90EE38588}">
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -10099,4 +10179,1480 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4418AB-7087-489E-B717-DDAB43816858}">
+  <dimension ref="A1:G63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11">
+        <v>250</v>
+      </c>
+      <c r="G2" s="11">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" s="10">
+        <v>100</v>
+      </c>
+      <c r="F3" s="11">
+        <v>250</v>
+      </c>
+      <c r="G3" s="11">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>350</v>
+      </c>
+      <c r="G4" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="10">
+        <v>100</v>
+      </c>
+      <c r="F5" s="11">
+        <v>350</v>
+      </c>
+      <c r="G5" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
+        <v>450</v>
+      </c>
+      <c r="G6" s="11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="10">
+        <v>100</v>
+      </c>
+      <c r="F7" s="11">
+        <v>450</v>
+      </c>
+      <c r="G7" s="11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8">
+        <v>250</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>280</v>
+      </c>
+      <c r="G8" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9">
+        <v>250</v>
+      </c>
+      <c r="E9" s="10">
+        <v>8</v>
+      </c>
+      <c r="F9" s="11">
+        <v>280</v>
+      </c>
+      <c r="G9" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10">
+        <v>250</v>
+      </c>
+      <c r="E10" s="10">
+        <v>8.01</v>
+      </c>
+      <c r="F10" s="11">
+        <v>260</v>
+      </c>
+      <c r="G10" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11">
+        <v>250</v>
+      </c>
+      <c r="E11" s="10">
+        <v>12</v>
+      </c>
+      <c r="F11" s="11">
+        <v>260</v>
+      </c>
+      <c r="G11" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12">
+        <v>250</v>
+      </c>
+      <c r="E12" s="10">
+        <v>12.01</v>
+      </c>
+      <c r="F12" s="11">
+        <v>250</v>
+      </c>
+      <c r="G12" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13">
+        <v>250</v>
+      </c>
+      <c r="E13" s="10">
+        <v>50</v>
+      </c>
+      <c r="F13" s="11">
+        <v>250</v>
+      </c>
+      <c r="G13" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14">
+        <v>250</v>
+      </c>
+      <c r="E14" s="10">
+        <v>50.01</v>
+      </c>
+      <c r="F14" s="11">
+        <v>240</v>
+      </c>
+      <c r="G14" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15">
+        <v>250</v>
+      </c>
+      <c r="E15" s="10">
+        <v>80</v>
+      </c>
+      <c r="F15" s="11">
+        <v>240</v>
+      </c>
+      <c r="G15" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16">
+        <v>250</v>
+      </c>
+      <c r="E16" s="10">
+        <v>80.010000000000005</v>
+      </c>
+      <c r="F16" s="11">
+        <v>230</v>
+      </c>
+      <c r="G16" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17">
+        <v>250</v>
+      </c>
+      <c r="E17" s="10">
+        <v>150</v>
+      </c>
+      <c r="F17" s="11">
+        <v>230</v>
+      </c>
+      <c r="G17" s="11">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18">
+        <v>200</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
+        <v>200</v>
+      </c>
+      <c r="G18" s="11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19">
+        <v>200</v>
+      </c>
+      <c r="E19" s="10">
+        <v>12</v>
+      </c>
+      <c r="F19" s="11">
+        <v>200</v>
+      </c>
+      <c r="G19" s="11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20">
+        <v>300</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>320</v>
+      </c>
+      <c r="G20" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21">
+        <v>300</v>
+      </c>
+      <c r="E21" s="10">
+        <v>8</v>
+      </c>
+      <c r="F21" s="11">
+        <v>320</v>
+      </c>
+      <c r="G21" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22">
+        <v>300</v>
+      </c>
+      <c r="E22" s="10">
+        <v>8.01</v>
+      </c>
+      <c r="F22" s="11">
+        <v>310</v>
+      </c>
+      <c r="G22" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23">
+        <v>300</v>
+      </c>
+      <c r="E23" s="10">
+        <v>12</v>
+      </c>
+      <c r="F23" s="11">
+        <v>310</v>
+      </c>
+      <c r="G23" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24">
+        <v>300</v>
+      </c>
+      <c r="E24" s="10">
+        <v>12.01</v>
+      </c>
+      <c r="F24" s="11">
+        <v>300</v>
+      </c>
+      <c r="G24" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25">
+        <v>300</v>
+      </c>
+      <c r="E25" s="10">
+        <v>20</v>
+      </c>
+      <c r="F25" s="11">
+        <v>300</v>
+      </c>
+      <c r="G25" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26">
+        <v>300</v>
+      </c>
+      <c r="E26" s="10">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="F26" s="11">
+        <v>280</v>
+      </c>
+      <c r="G26" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27">
+        <v>300</v>
+      </c>
+      <c r="E27" s="10">
+        <v>50</v>
+      </c>
+      <c r="F27" s="11">
+        <v>280</v>
+      </c>
+      <c r="G27" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28">
+        <v>300</v>
+      </c>
+      <c r="E28" s="10">
+        <v>50.01</v>
+      </c>
+      <c r="F28" s="11">
+        <v>270</v>
+      </c>
+      <c r="G28" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29">
+        <v>300</v>
+      </c>
+      <c r="E29" s="10">
+        <v>80</v>
+      </c>
+      <c r="F29" s="11">
+        <v>270</v>
+      </c>
+      <c r="G29" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30">
+        <v>300</v>
+      </c>
+      <c r="E30" s="10">
+        <v>80.010000000000005</v>
+      </c>
+      <c r="F30" s="11">
+        <v>260</v>
+      </c>
+      <c r="G30" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C31" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31">
+        <v>300</v>
+      </c>
+      <c r="E31" s="10">
+        <v>150</v>
+      </c>
+      <c r="F31" s="11">
+        <v>260</v>
+      </c>
+      <c r="G31" s="11">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32">
+        <v>350</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0</v>
+      </c>
+      <c r="F32" s="11">
+        <v>360</v>
+      </c>
+      <c r="G32" s="11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33">
+        <v>350</v>
+      </c>
+      <c r="E33" s="10">
+        <v>12</v>
+      </c>
+      <c r="F33" s="11">
+        <v>360</v>
+      </c>
+      <c r="G33" s="11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34">
+        <v>350</v>
+      </c>
+      <c r="E34" s="10">
+        <v>12.01</v>
+      </c>
+      <c r="F34" s="11">
+        <v>350</v>
+      </c>
+      <c r="G34" s="11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35">
+        <v>350</v>
+      </c>
+      <c r="E35" s="10">
+        <v>20</v>
+      </c>
+      <c r="F35" s="11">
+        <v>350</v>
+      </c>
+      <c r="G35" s="11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36">
+        <v>350</v>
+      </c>
+      <c r="E36" s="10">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="F36" s="11">
+        <v>340</v>
+      </c>
+      <c r="G36" s="11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>153</v>
+      </c>
+      <c r="B37" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37">
+        <v>350</v>
+      </c>
+      <c r="E37" s="10">
+        <v>80</v>
+      </c>
+      <c r="F37" s="11">
+        <v>340</v>
+      </c>
+      <c r="G37" s="11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38">
+        <v>350</v>
+      </c>
+      <c r="E38" s="10">
+        <v>80.010000000000005</v>
+      </c>
+      <c r="F38" s="11">
+        <v>330</v>
+      </c>
+      <c r="G38" s="11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39">
+        <v>350</v>
+      </c>
+      <c r="E39" s="10">
+        <v>150</v>
+      </c>
+      <c r="F39" s="11">
+        <v>330</v>
+      </c>
+      <c r="G39" s="11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40">
+        <v>400</v>
+      </c>
+      <c r="E40" s="10">
+        <v>0</v>
+      </c>
+      <c r="F40" s="11">
+        <v>400</v>
+      </c>
+      <c r="G40" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41">
+        <v>400</v>
+      </c>
+      <c r="E41" s="10">
+        <v>12</v>
+      </c>
+      <c r="F41" s="11">
+        <v>400</v>
+      </c>
+      <c r="G41" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42">
+        <v>400</v>
+      </c>
+      <c r="E42" s="10">
+        <v>12.01</v>
+      </c>
+      <c r="F42" s="11">
+        <v>380</v>
+      </c>
+      <c r="G42" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" t="s">
+        <v>160</v>
+      </c>
+      <c r="C43" t="s">
+        <v>157</v>
+      </c>
+      <c r="D43">
+        <v>400</v>
+      </c>
+      <c r="E43" s="10">
+        <v>20</v>
+      </c>
+      <c r="F43" s="11">
+        <v>380</v>
+      </c>
+      <c r="G43" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44">
+        <v>400</v>
+      </c>
+      <c r="E44" s="10">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="F44" s="11">
+        <v>360</v>
+      </c>
+      <c r="G44" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" t="s">
+        <v>157</v>
+      </c>
+      <c r="D45">
+        <v>400</v>
+      </c>
+      <c r="E45" s="10">
+        <v>80</v>
+      </c>
+      <c r="F45" s="11">
+        <v>360</v>
+      </c>
+      <c r="G45" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46">
+        <v>450</v>
+      </c>
+      <c r="E46" s="10">
+        <v>0</v>
+      </c>
+      <c r="F46" s="11">
+        <v>450</v>
+      </c>
+      <c r="G46" s="11">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B47" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47">
+        <v>450</v>
+      </c>
+      <c r="E47" s="10">
+        <v>20</v>
+      </c>
+      <c r="F47" s="11">
+        <v>450</v>
+      </c>
+      <c r="G47" s="11">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48">
+        <v>450</v>
+      </c>
+      <c r="E48" s="10">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="F48" s="11">
+        <v>420</v>
+      </c>
+      <c r="G48" s="11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49" t="s">
+        <v>157</v>
+      </c>
+      <c r="D49">
+        <v>450</v>
+      </c>
+      <c r="E49" s="10">
+        <v>32</v>
+      </c>
+      <c r="F49" s="11">
+        <v>420</v>
+      </c>
+      <c r="G49" s="11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" t="s">
+        <v>157</v>
+      </c>
+      <c r="D50">
+        <v>450</v>
+      </c>
+      <c r="E50" s="10">
+        <v>32.01</v>
+      </c>
+      <c r="F50" s="11">
+        <v>400</v>
+      </c>
+      <c r="G50" s="11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51">
+        <v>450</v>
+      </c>
+      <c r="E51" s="10">
+        <v>50</v>
+      </c>
+      <c r="F51" s="11">
+        <v>400</v>
+      </c>
+      <c r="G51" s="11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" t="s">
+        <v>158</v>
+      </c>
+      <c r="D52">
+        <v>350</v>
+      </c>
+      <c r="E52" s="10">
+        <v>0</v>
+      </c>
+      <c r="F52" s="11">
+        <v>360</v>
+      </c>
+      <c r="G52" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" t="s">
+        <v>160</v>
+      </c>
+      <c r="C53" t="s">
+        <v>158</v>
+      </c>
+      <c r="D53">
+        <v>350</v>
+      </c>
+      <c r="E53" s="10">
+        <v>11</v>
+      </c>
+      <c r="F53" s="11">
+        <v>360</v>
+      </c>
+      <c r="G53" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" t="s">
+        <v>158</v>
+      </c>
+      <c r="D54">
+        <v>350</v>
+      </c>
+      <c r="E54" s="10">
+        <v>11.01</v>
+      </c>
+      <c r="F54" s="11">
+        <v>340</v>
+      </c>
+      <c r="G54" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55">
+        <v>350</v>
+      </c>
+      <c r="E55" s="10">
+        <v>40</v>
+      </c>
+      <c r="F55" s="11">
+        <v>340</v>
+      </c>
+      <c r="G55" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" t="s">
+        <v>158</v>
+      </c>
+      <c r="D56">
+        <v>350</v>
+      </c>
+      <c r="E56" s="10">
+        <v>40.01</v>
+      </c>
+      <c r="F56" s="11">
+        <v>330</v>
+      </c>
+      <c r="G56" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" t="s">
+        <v>160</v>
+      </c>
+      <c r="C57" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57">
+        <v>350</v>
+      </c>
+      <c r="E57" s="10">
+        <v>100</v>
+      </c>
+      <c r="F57" s="11">
+        <v>330</v>
+      </c>
+      <c r="G57" s="11">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>154</v>
+      </c>
+      <c r="B58" t="s">
+        <v>160</v>
+      </c>
+      <c r="C58" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58">
+        <v>300</v>
+      </c>
+      <c r="E58" s="10">
+        <v>0</v>
+      </c>
+      <c r="F58" s="11">
+        <v>320</v>
+      </c>
+      <c r="G58" s="11">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59">
+        <v>300</v>
+      </c>
+      <c r="E59" s="10">
+        <v>11</v>
+      </c>
+      <c r="F59" s="11">
+        <v>320</v>
+      </c>
+      <c r="G59" s="11">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60" t="s">
+        <v>160</v>
+      </c>
+      <c r="C60" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60">
+        <v>300</v>
+      </c>
+      <c r="E60" s="10">
+        <v>11.01</v>
+      </c>
+      <c r="F60" s="11">
+        <v>300</v>
+      </c>
+      <c r="G60" s="11">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" t="s">
+        <v>158</v>
+      </c>
+      <c r="D61">
+        <v>300</v>
+      </c>
+      <c r="E61" s="10">
+        <v>17</v>
+      </c>
+      <c r="F61" s="11">
+        <v>300</v>
+      </c>
+      <c r="G61" s="11">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>154</v>
+      </c>
+      <c r="B62" t="s">
+        <v>160</v>
+      </c>
+      <c r="C62" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62">
+        <v>300</v>
+      </c>
+      <c r="E62" s="10">
+        <v>17.010000000000002</v>
+      </c>
+      <c r="F62" s="11">
+        <v>280</v>
+      </c>
+      <c r="G62" s="11">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" t="s">
+        <v>160</v>
+      </c>
+      <c r="C63" t="s">
+        <v>158</v>
+      </c>
+      <c r="D63">
+        <v>300</v>
+      </c>
+      <c r="E63" s="10">
+        <v>100</v>
+      </c>
+      <c r="F63" s="11">
+        <v>280</v>
+      </c>
+      <c r="G63" s="11">
+        <v>440</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update units for steel grades.
</commit_message>
<xml_diff>
--- a/data/steel_data.xlsx
+++ b/data/steel_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D39C5A-149F-463E-82AC-CDDD4337E87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7AB3A6-5370-4904-A31B-1443A056F6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
   </bookViews>
@@ -410,9 +410,6 @@
     <t>mass</t>
   </si>
   <si>
-    <t>section_type</t>
-  </si>
-  <si>
     <t>fabrication_type</t>
   </si>
   <si>
@@ -519,6 +516,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>section_shape</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
     <numFmt numFmtId="168" formatCode="##0.00E+00&quot; m⁴&quot;"/>
     <numFmt numFmtId="169" formatCode="##0.00E+00&quot; m³&quot;"/>
     <numFmt numFmtId="170" formatCode="##0.00E+00&quot; m⁶&quot;"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -594,17 +594,17 @@
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="55">
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.0"/>
+      <numFmt numFmtId="171" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.0"/>
+      <numFmt numFmtId="171" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1908,7 +1908,7 @@
     <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="49"/>
     <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="48"/>
     <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_type" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="46"/>
     <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="45"/>
     <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="44"/>
     <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="43"/>
@@ -1942,7 +1942,7 @@
     <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="23"/>
     <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_type" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="21"/>
     <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="20"/>
     <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="19"/>
     <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="18"/>
@@ -2282,7 +2282,7 @@
   <dimension ref="A1:W100"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,64 +2315,64 @@
         <v>123</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -9402,7 +9402,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9435,61 +9435,61 @@
         <v>123</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="Q1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -10185,8 +10185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4418AB-7087-489E-B717-DDAB43816858}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10202,39 +10202,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
         <v>146</v>
       </c>
-      <c r="B1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" t="s">
         <v>147</v>
-      </c>
-      <c r="E1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
@@ -10248,19 +10248,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="10">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="F3" s="11">
         <v>250</v>
@@ -10271,16 +10271,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
@@ -10294,19 +10294,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="10">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="F5" s="11">
         <v>350</v>
@@ -10317,16 +10317,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E6" s="10">
         <v>0</v>
@@ -10340,19 +10340,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="10">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="F7" s="11">
         <v>450</v>
@@ -10363,13 +10363,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8">
         <v>250</v>
@@ -10386,19 +10386,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9">
         <v>250</v>
       </c>
       <c r="E9" s="10">
-        <v>8</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F9" s="11">
         <v>280</v>
@@ -10409,19 +10409,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10">
         <v>250</v>
       </c>
       <c r="E10" s="10">
-        <v>8.01</v>
+        <v>8.0099999999999998E-3</v>
       </c>
       <c r="F10" s="11">
         <v>260</v>
@@ -10432,19 +10432,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D11">
         <v>250</v>
       </c>
       <c r="E11" s="10">
-        <v>12</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F11" s="11">
         <v>260</v>
@@ -10455,19 +10455,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12">
         <v>250</v>
       </c>
       <c r="E12" s="10">
-        <v>12.01</v>
+        <v>1.201E-2</v>
       </c>
       <c r="F12" s="11">
         <v>250</v>
@@ -10478,19 +10478,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13">
         <v>250</v>
       </c>
       <c r="E13" s="10">
-        <v>50</v>
+        <v>0.05</v>
       </c>
       <c r="F13" s="11">
         <v>250</v>
@@ -10501,19 +10501,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14">
         <v>250</v>
       </c>
       <c r="E14" s="10">
-        <v>50.01</v>
+        <v>5.0009999999999999E-2</v>
       </c>
       <c r="F14" s="11">
         <v>240</v>
@@ -10524,19 +10524,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D15">
         <v>250</v>
       </c>
       <c r="E15" s="10">
-        <v>80</v>
+        <v>0.08</v>
       </c>
       <c r="F15" s="11">
         <v>240</v>
@@ -10547,19 +10547,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16">
         <v>250</v>
       </c>
       <c r="E16" s="10">
-        <v>80.010000000000005</v>
+        <v>8.0010000000000012E-2</v>
       </c>
       <c r="F16" s="11">
         <v>230</v>
@@ -10570,19 +10570,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D17">
         <v>250</v>
       </c>
       <c r="E17" s="10">
-        <v>150</v>
+        <v>0.15</v>
       </c>
       <c r="F17" s="11">
         <v>230</v>
@@ -10593,13 +10593,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D18">
         <v>200</v>
@@ -10616,19 +10616,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D19">
         <v>200</v>
       </c>
       <c r="E19" s="10">
-        <v>12</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F19" s="11">
         <v>200</v>
@@ -10639,13 +10639,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D20">
         <v>300</v>
@@ -10662,19 +10662,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D21">
         <v>300</v>
       </c>
       <c r="E21" s="10">
-        <v>8</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F21" s="11">
         <v>320</v>
@@ -10685,19 +10685,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22">
         <v>300</v>
       </c>
       <c r="E22" s="10">
-        <v>8.01</v>
+        <v>8.0099999999999998E-3</v>
       </c>
       <c r="F22" s="11">
         <v>310</v>
@@ -10708,19 +10708,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D23">
         <v>300</v>
       </c>
       <c r="E23" s="10">
-        <v>12</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F23" s="11">
         <v>310</v>
@@ -10731,19 +10731,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D24">
         <v>300</v>
       </c>
       <c r="E24" s="10">
-        <v>12.01</v>
+        <v>1.201E-2</v>
       </c>
       <c r="F24" s="11">
         <v>300</v>
@@ -10754,19 +10754,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D25">
         <v>300</v>
       </c>
       <c r="E25" s="10">
-        <v>20</v>
+        <v>0.02</v>
       </c>
       <c r="F25" s="11">
         <v>300</v>
@@ -10777,19 +10777,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D26">
         <v>300</v>
       </c>
       <c r="E26" s="10">
-        <v>20.010000000000002</v>
+        <v>2.001E-2</v>
       </c>
       <c r="F26" s="11">
         <v>280</v>
@@ -10800,19 +10800,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D27">
         <v>300</v>
       </c>
       <c r="E27" s="10">
-        <v>50</v>
+        <v>0.05</v>
       </c>
       <c r="F27" s="11">
         <v>280</v>
@@ -10823,19 +10823,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D28">
         <v>300</v>
       </c>
       <c r="E28" s="10">
-        <v>50.01</v>
+        <v>5.0009999999999999E-2</v>
       </c>
       <c r="F28" s="11">
         <v>270</v>
@@ -10846,19 +10846,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D29">
         <v>300</v>
       </c>
       <c r="E29" s="10">
-        <v>80</v>
+        <v>0.08</v>
       </c>
       <c r="F29" s="11">
         <v>270</v>
@@ -10869,19 +10869,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D30">
         <v>300</v>
       </c>
       <c r="E30" s="10">
-        <v>80.010000000000005</v>
+        <v>8.0010000000000012E-2</v>
       </c>
       <c r="F30" s="11">
         <v>260</v>
@@ -10892,19 +10892,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D31">
         <v>300</v>
       </c>
       <c r="E31" s="10">
-        <v>150</v>
+        <v>0.15</v>
       </c>
       <c r="F31" s="11">
         <v>260</v>
@@ -10915,13 +10915,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D32">
         <v>350</v>
@@ -10938,19 +10938,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D33">
         <v>350</v>
       </c>
       <c r="E33" s="10">
-        <v>12</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F33" s="11">
         <v>360</v>
@@ -10961,19 +10961,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D34">
         <v>350</v>
       </c>
       <c r="E34" s="10">
-        <v>12.01</v>
+        <v>1.201E-2</v>
       </c>
       <c r="F34" s="11">
         <v>350</v>
@@ -10984,19 +10984,19 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D35">
         <v>350</v>
       </c>
       <c r="E35" s="10">
-        <v>20</v>
+        <v>0.02</v>
       </c>
       <c r="F35" s="11">
         <v>350</v>
@@ -11007,19 +11007,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D36">
         <v>350</v>
       </c>
       <c r="E36" s="10">
-        <v>20.010000000000002</v>
+        <v>2.001E-2</v>
       </c>
       <c r="F36" s="11">
         <v>340</v>
@@ -11030,19 +11030,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D37">
         <v>350</v>
       </c>
       <c r="E37" s="10">
-        <v>80</v>
+        <v>0.08</v>
       </c>
       <c r="F37" s="11">
         <v>340</v>
@@ -11053,19 +11053,19 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D38">
         <v>350</v>
       </c>
       <c r="E38" s="10">
-        <v>80.010000000000005</v>
+        <v>8.0010000000000012E-2</v>
       </c>
       <c r="F38" s="11">
         <v>330</v>
@@ -11076,19 +11076,19 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D39">
         <v>350</v>
       </c>
       <c r="E39" s="10">
-        <v>150</v>
+        <v>0.15</v>
       </c>
       <c r="F39" s="11">
         <v>330</v>
@@ -11099,13 +11099,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D40">
         <v>400</v>
@@ -11122,19 +11122,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D41">
         <v>400</v>
       </c>
       <c r="E41" s="10">
-        <v>12</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F41" s="11">
         <v>400</v>
@@ -11145,19 +11145,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D42">
         <v>400</v>
       </c>
       <c r="E42" s="10">
-        <v>12.01</v>
+        <v>1.201E-2</v>
       </c>
       <c r="F42" s="11">
         <v>380</v>
@@ -11168,19 +11168,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D43">
         <v>400</v>
       </c>
       <c r="E43" s="10">
-        <v>20</v>
+        <v>0.02</v>
       </c>
       <c r="F43" s="11">
         <v>380</v>
@@ -11191,19 +11191,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D44">
         <v>400</v>
       </c>
       <c r="E44" s="10">
-        <v>20.010000000000002</v>
+        <v>2.001E-2</v>
       </c>
       <c r="F44" s="11">
         <v>360</v>
@@ -11214,19 +11214,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D45">
         <v>400</v>
       </c>
       <c r="E45" s="10">
-        <v>80</v>
+        <v>0.08</v>
       </c>
       <c r="F45" s="11">
         <v>360</v>
@@ -11237,13 +11237,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D46">
         <v>450</v>
@@ -11260,19 +11260,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D47">
         <v>450</v>
       </c>
       <c r="E47" s="10">
-        <v>20</v>
+        <v>0.02</v>
       </c>
       <c r="F47" s="11">
         <v>450</v>
@@ -11283,19 +11283,19 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D48">
         <v>450</v>
       </c>
       <c r="E48" s="10">
-        <v>20.010000000000002</v>
+        <v>2.001E-2</v>
       </c>
       <c r="F48" s="11">
         <v>420</v>
@@ -11306,19 +11306,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D49">
         <v>450</v>
       </c>
       <c r="E49" s="10">
-        <v>32</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="F49" s="11">
         <v>420</v>
@@ -11329,19 +11329,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D50">
         <v>450</v>
       </c>
       <c r="E50" s="10">
-        <v>32.01</v>
+        <v>3.2009999999999997E-2</v>
       </c>
       <c r="F50" s="11">
         <v>400</v>
@@ -11352,19 +11352,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D51">
         <v>450</v>
       </c>
       <c r="E51" s="10">
-        <v>50</v>
+        <v>0.05</v>
       </c>
       <c r="F51" s="11">
         <v>400</v>
@@ -11375,13 +11375,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D52">
         <v>350</v>
@@ -11398,19 +11398,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D53">
         <v>350</v>
       </c>
       <c r="E53" s="10">
-        <v>11</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F53" s="11">
         <v>360</v>
@@ -11421,19 +11421,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D54">
         <v>350</v>
       </c>
       <c r="E54" s="10">
-        <v>11.01</v>
+        <v>1.1009999999999999E-2</v>
       </c>
       <c r="F54" s="11">
         <v>340</v>
@@ -11444,19 +11444,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B55" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C55" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D55">
         <v>350</v>
       </c>
       <c r="E55" s="10">
-        <v>40</v>
+        <v>0.04</v>
       </c>
       <c r="F55" s="11">
         <v>340</v>
@@ -11467,19 +11467,19 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D56">
         <v>350</v>
       </c>
       <c r="E56" s="10">
-        <v>40.01</v>
+        <v>4.0009999999999997E-2</v>
       </c>
       <c r="F56" s="11">
         <v>330</v>
@@ -11490,19 +11490,19 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D57">
         <v>350</v>
       </c>
       <c r="E57" s="10">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="F57" s="11">
         <v>330</v>
@@ -11513,13 +11513,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D58">
         <v>300</v>
@@ -11536,19 +11536,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D59">
         <v>300</v>
       </c>
       <c r="E59" s="10">
-        <v>11</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F59" s="11">
         <v>320</v>
@@ -11559,19 +11559,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D60">
         <v>300</v>
       </c>
       <c r="E60" s="10">
-        <v>11.01</v>
+        <v>1.1009999999999999E-2</v>
       </c>
       <c r="F60" s="11">
         <v>300</v>
@@ -11582,19 +11582,19 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C61" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D61">
         <v>300</v>
       </c>
       <c r="E61" s="10">
-        <v>17</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="F61" s="11">
         <v>300</v>
@@ -11605,19 +11605,19 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D62">
         <v>300</v>
       </c>
       <c r="E62" s="10">
-        <v>17.010000000000002</v>
+        <v>1.7010000000000001E-2</v>
       </c>
       <c r="F62" s="11">
         <v>280</v>
@@ -11628,19 +11628,19 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D63">
         <v>300</v>
       </c>
       <c r="E63" s="10">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="F63" s="11">
         <v>280</v>

</xml_diff>

<commit_message>
update steel data and add d_1 into section_df methods.
</commit_message>
<xml_diff>
--- a/data/steel_data.xlsx
+++ b/data/steel_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4C1A00-6FE9-4CF5-903D-295B5AF3ED67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F678EBC6-C156-4D2A-8E38-F9A35D457728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t/>
   </si>
   <si>
-    <t>Hot Rolled</t>
-  </si>
-  <si>
     <t>125PFC</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>WB</t>
   </si>
   <si>
-    <t>Welded</t>
-  </si>
-  <si>
     <t>1000WB258</t>
   </si>
   <si>
@@ -522,6 +516,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>hot rolled</t>
+  </si>
+  <si>
+    <t>welded</t>
   </si>
 </sst>
 </file>
@@ -603,43 +603,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="57">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF404041"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF404041"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00&quot; kg / m&quot;"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="171" formatCode="0.0"/>
     </dxf>
@@ -1172,6 +1135,25 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF404041"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00&quot; kg / m&quot;"/>
     </dxf>
     <dxf>
       <font>
@@ -1809,6 +1791,24 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF404041"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1946,63 +1946,63 @@
   <autoFilter ref="A1:X100" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="51"/>
-    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="44"/>
-    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="43"/>
-    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="41"/>
-    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="40">
+    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="43"/>
+    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="42"/>
+    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="39">
       <calculatedColumnFormula>IF(Table2[[#This Row],[w_1]]="",Table2[[#This Row],[r_1]],Table2[[#This Row],[w_1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="39"/>
-    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="38"/>
-    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="37"/>
-    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="36"/>
-    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="35"/>
-    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="34"/>
-    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="33"/>
-    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="32"/>
-    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="31"/>
-    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="30"/>
-    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="29"/>
+    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="38"/>
+    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="37"/>
+    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="36"/>
+    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="35"/>
+    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="34"/>
+    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="33"/>
+    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="32"/>
+    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="31"/>
+    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="30"/>
+    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="29"/>
+    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:W11" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="17"/>
-    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="16"/>
-    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="15"/>
-    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="14"/>
-    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="13"/>
-    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="12"/>
-    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="11"/>
-    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="10"/>
-    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="9"/>
-    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="8"/>
-    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="7"/>
-    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="6"/>
-    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="15"/>
+    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="14"/>
+    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="13"/>
+    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="12"/>
+    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="11"/>
+    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="10"/>
+    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="9"/>
+    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="8"/>
+    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="7"/>
+    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="6"/>
+    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="5"/>
+    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="4"/>
+    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2016,9 +2016,9 @@
     <tableColumn id="7" xr3:uid="{F4DBA019-F123-4B98-A615-C1C293EAF7F6}" name="current"/>
     <tableColumn id="6" xr3:uid="{49F22BD6-5E2F-4DCD-B8F2-753E49B729CD}" name="form"/>
     <tableColumn id="2" xr3:uid="{D21D031E-2102-48DD-8FDF-9B85CD1F2DC4}" name="grade"/>
-    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2323,8 +2323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DE0702-9028-4C23-A846-1BC90EE38588}">
   <dimension ref="A1:X100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,96 +2349,96 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="3">
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G2" s="5">
         <v>0.15</v>
@@ -2496,22 +2496,22 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3">
         <v>18</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G3" s="5">
         <v>0.155</v>
@@ -2569,22 +2569,22 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3">
         <v>16.100000000000001</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G4" s="5">
         <v>0.17299999999999999</v>
@@ -2642,22 +2642,22 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3">
         <v>18.100000000000001</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G5" s="5">
         <v>0.17499999999999999</v>
@@ -2715,22 +2715,22 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
         <v>22.2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G6" s="5">
         <v>0.17899999999999999</v>
@@ -2788,22 +2788,22 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3">
         <v>18.2</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G7" s="5">
         <v>0.19800000000000001</v>
@@ -2861,22 +2861,22 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
         <v>22.3</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G8" s="5">
         <v>0.20200000000000001</v>
@@ -2934,22 +2934,22 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3">
         <v>25.4</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G9" s="5">
         <v>0.20300000000000001</v>
@@ -3007,22 +3007,22 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3">
         <v>29.8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G10" s="5">
         <v>0.20699999999999999</v>
@@ -3080,22 +3080,22 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3">
         <v>25.7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G11" s="5">
         <v>0.248</v>
@@ -3153,22 +3153,22 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3">
         <v>31.4</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G12" s="5">
         <v>0.252</v>
@@ -3226,22 +3226,22 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3">
         <v>37.299999999999997</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G13" s="5">
         <v>0.25600000000000001</v>
@@ -3299,22 +3299,22 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3">
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G14" s="5">
         <v>0.29799999999999999</v>
@@ -3372,22 +3372,22 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="3">
         <v>40.4</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G15" s="5">
         <v>0.30399999999999999</v>
@@ -3445,22 +3445,22 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3">
         <v>46.2</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G16" s="5">
         <v>0.307</v>
@@ -3518,22 +3518,22 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="3">
         <v>44.7</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G17" s="5">
         <v>0.35199999999999998</v>
@@ -3591,22 +3591,22 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="3">
         <v>50.7</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G18" s="5">
         <v>0.35599999999999998</v>
@@ -3664,22 +3664,22 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="3">
         <v>56.7</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G19" s="5">
         <v>0.35899999999999999</v>
@@ -3737,22 +3737,22 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="3">
         <v>53.7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G20" s="5">
         <v>0.40300000000000002</v>
@@ -3810,22 +3810,22 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="3">
         <v>59.7</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G21" s="5">
         <v>0.40600000000000003</v>
@@ -3883,22 +3883,22 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="3">
         <v>67.099999999999994</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G22" s="5">
         <v>0.45400000000000001</v>
@@ -3956,22 +3956,22 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="3">
         <v>74.599999999999994</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G23" s="5">
         <v>0.45700000000000002</v>
@@ -4029,22 +4029,22 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="3">
         <v>82.1</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G24" s="5">
         <v>0.46</v>
@@ -4102,22 +4102,22 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="3">
         <v>82</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G25" s="5">
         <v>0.52800000000000002</v>
@@ -4175,22 +4175,22 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="3">
         <v>92.4</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G26" s="5">
         <v>0.53300000000000003</v>
@@ -4248,22 +4248,22 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" s="3">
         <v>101</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G27" s="5">
         <v>0.60199999999999998</v>
@@ -4321,22 +4321,22 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="3">
         <v>113</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G28" s="5">
         <v>0.60699999999999998</v>
@@ -4394,22 +4394,22 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="3">
         <v>125</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G29" s="5">
         <v>0.61199999999999999</v>
@@ -4467,22 +4467,22 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" s="3">
         <v>125</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G30" s="5">
         <v>0.67800000000000005</v>
@@ -4540,22 +4540,22 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" s="3">
         <v>140</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G31" s="5">
         <v>0.68400000000000005</v>
@@ -4613,22 +4613,22 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" s="3">
         <v>147</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G32" s="5">
         <v>0.754</v>
@@ -4686,22 +4686,22 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="3">
         <v>173</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G33" s="5">
         <v>0.76200000000000001</v>
@@ -4759,22 +4759,22 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34" s="3">
         <v>197</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G34" s="5">
         <v>0.77</v>
@@ -4832,22 +4832,22 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D35" s="3">
         <v>220</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G35" s="5">
         <v>0.77500000000000002</v>
@@ -4905,22 +4905,22 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" s="3">
         <v>244</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G36" s="5">
         <v>0.78100000000000003</v>
@@ -4978,22 +4978,22 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="D37" s="3">
         <v>122</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G37" s="5">
         <v>0.23</v>
@@ -5051,22 +5051,22 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D38" s="3">
         <v>146</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G38" s="5">
         <v>0.245</v>
@@ -5124,22 +5124,22 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D39" s="3">
         <v>62.6</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G39" s="5">
         <v>0.247</v>
@@ -5197,22 +5197,22 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" s="3">
         <v>84.9</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G40" s="5">
         <v>0.254</v>
@@ -5270,22 +5270,22 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D41" s="3">
         <v>110</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G41" s="5">
         <v>0.308</v>
@@ -5343,22 +5343,22 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D42" s="3">
         <v>149</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G42" s="5">
         <v>0.318</v>
@@ -5416,22 +5416,22 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" s="3">
         <v>78.8</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G43" s="5">
         <v>0.29899999999999999</v>
@@ -5489,22 +5489,22 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="D44" s="3">
         <v>14.8</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G44" s="5">
         <v>9.7000000000000003E-2</v>
@@ -5562,22 +5562,22 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D45" s="3">
         <v>23.4</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G45" s="5">
         <v>0.152</v>
@@ -5635,22 +5635,22 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D46" s="3">
         <v>30</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G46" s="5">
         <v>0.158</v>
@@ -5708,22 +5708,22 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D47" s="3">
         <v>37.200000000000003</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G47" s="5">
         <v>0.16200000000000001</v>
@@ -5781,22 +5781,22 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48" s="3">
         <v>46.2</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G48" s="5">
         <v>0.20300000000000001</v>
@@ -5854,22 +5854,22 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D49" s="3">
         <v>52.2</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G49" s="5">
         <v>0.20599999999999999</v>
@@ -5927,22 +5927,22 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D50" s="3">
         <v>59.3</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G50" s="5">
         <v>0.21</v>
@@ -6000,22 +6000,22 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D51" s="3">
         <v>72.900000000000006</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G51" s="5">
         <v>0.254</v>
@@ -6073,22 +6073,22 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D52" s="3">
         <v>89.5</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G52" s="5">
         <v>0.26</v>
@@ -6146,22 +6146,22 @@
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D53" s="3">
         <v>118</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G53" s="5">
         <v>0.315</v>
@@ -6219,22 +6219,22 @@
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D54" s="3">
         <v>137</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G54" s="5">
         <v>0.32100000000000001</v>
@@ -6292,22 +6292,22 @@
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D55" s="3">
         <v>158</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G55" s="5">
         <v>0.32700000000000001</v>
@@ -6365,22 +6365,22 @@
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D56" s="3">
         <v>198</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G56" s="5">
         <v>0.34</v>
@@ -6438,22 +6438,22 @@
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D57" s="3">
         <v>240</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G57" s="5">
         <v>0.35299999999999998</v>
@@ -6511,22 +6511,22 @@
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D58" s="3">
         <v>283</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G58" s="5">
         <v>0.36499999999999999</v>
@@ -6584,22 +6584,22 @@
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D59" s="3">
         <v>96.8</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G59" s="5">
         <v>0.308</v>
@@ -6657,22 +6657,22 @@
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D60" s="3">
         <v>215</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G60" s="5">
         <v>1</v>
@@ -6732,22 +6732,22 @@
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D61" s="3">
         <v>258</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G61" s="5">
         <v>1.01</v>
@@ -6807,22 +6807,22 @@
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D62" s="3">
         <v>296</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G62" s="5">
         <v>1.016</v>
@@ -6882,22 +6882,22 @@
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D63" s="3">
         <v>322</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G63" s="5">
         <v>1.024</v>
@@ -6957,22 +6957,22 @@
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D64" s="3">
         <v>249</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G64" s="5">
         <v>1.17</v>
@@ -7032,22 +7032,22 @@
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D65" s="3">
         <v>278</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G65" s="5">
         <v>1.17</v>
@@ -7107,22 +7107,22 @@
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D66" s="3">
         <v>317</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G66" s="5">
         <v>1.1759999999999999</v>
@@ -7182,22 +7182,22 @@
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D67" s="3">
         <v>342</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G67" s="5">
         <v>1.1839999999999999</v>
@@ -7257,22 +7257,22 @@
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D68" s="3">
         <v>392</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G68" s="5">
         <v>1.1839999999999999</v>
@@ -7332,22 +7332,22 @@
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D69" s="3">
         <v>423</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G69" s="5">
         <v>1.1919999999999999</v>
@@ -7407,22 +7407,22 @@
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D70" s="3">
         <v>455</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G70" s="5">
         <v>1.2</v>
@@ -7482,22 +7482,22 @@
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D71" s="3">
         <v>115</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G71" s="5">
         <v>0.69199999999999995</v>
@@ -7557,22 +7557,22 @@
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D72" s="3">
         <v>130</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G72" s="5">
         <v>0.7</v>
@@ -7632,22 +7632,22 @@
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D73" s="3">
         <v>150</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G73" s="5">
         <v>0.71</v>
@@ -7707,22 +7707,22 @@
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D74" s="3">
         <v>173</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G74" s="5">
         <v>0.71599999999999997</v>
@@ -7782,22 +7782,22 @@
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D75" s="3">
         <v>122</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G75" s="5">
         <v>0.79200000000000004</v>
@@ -7857,22 +7857,22 @@
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D76" s="3">
         <v>146</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G76" s="5">
         <v>0.8</v>
@@ -7932,22 +7932,22 @@
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D77" s="3">
         <v>168</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G77" s="5">
         <v>0.81</v>
@@ -8007,22 +8007,22 @@
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D78" s="3">
         <v>192</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G78" s="5">
         <v>0.81599999999999995</v>
@@ -8082,22 +8082,22 @@
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D79" s="3">
         <v>175</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G79" s="5">
         <v>0.9</v>
@@ -8157,22 +8157,22 @@
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D80" s="3">
         <v>218</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G80" s="5">
         <v>0.91</v>
@@ -8232,22 +8232,22 @@
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D81" s="3">
         <v>257</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G81" s="5">
         <v>0.91600000000000004</v>
@@ -8307,22 +8307,22 @@
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D82" s="3">
         <v>282</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G82" s="5">
         <v>0.92400000000000004</v>
@@ -8382,22 +8382,22 @@
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D83" s="3">
         <v>197</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G83" s="5">
         <v>0.33100000000000002</v>
@@ -8457,22 +8457,22 @@
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D84" s="3">
         <v>230</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G84" s="5">
         <v>0.33900000000000002</v>
@@ -8532,22 +8532,22 @@
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D85" s="3">
         <v>258</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G85" s="5">
         <v>0.34699999999999998</v>
@@ -8607,22 +8607,22 @@
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D86" s="3">
         <v>280</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G86" s="5">
         <v>0.35499999999999998</v>
@@ -8682,22 +8682,22 @@
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D87" s="3">
         <v>144</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G87" s="5">
         <v>0.38200000000000001</v>
@@ -8757,22 +8757,22 @@
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D88" s="3">
         <v>181</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G88" s="5">
         <v>0.39</v>
@@ -8832,22 +8832,22 @@
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D89" s="3">
         <v>212</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G89" s="5">
         <v>0.4</v>
@@ -8907,22 +8907,22 @@
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D90" s="3">
         <v>270</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G90" s="5">
         <v>0.41399999999999998</v>
@@ -8982,22 +8982,22 @@
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D91" s="3">
         <v>303</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G91" s="5">
         <v>0.42199999999999999</v>
@@ -9057,22 +9057,22 @@
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D92" s="3">
         <v>328</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G92" s="5">
         <v>0.43</v>
@@ -9132,22 +9132,22 @@
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D93" s="3">
         <v>361</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G93" s="5">
         <v>0.43</v>
@@ -9207,22 +9207,22 @@
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D94" s="3">
         <v>228</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G94" s="5">
         <v>0.49</v>
@@ -9282,22 +9282,22 @@
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D95" s="3">
         <v>267</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G95" s="5">
         <v>0.5</v>
@@ -9357,22 +9357,22 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D96" s="3">
         <v>290</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G96" s="5">
         <v>0.50600000000000001</v>
@@ -9432,22 +9432,22 @@
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D97" s="3">
         <v>340</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G97" s="5">
         <v>0.51400000000000001</v>
@@ -9507,22 +9507,22 @@
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D98" s="3">
         <v>383</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G98" s="5">
         <v>0.47199999999999998</v>
@@ -9582,22 +9582,22 @@
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D99" s="3">
         <v>414</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G99" s="5">
         <v>0.48</v>
@@ -9657,22 +9657,22 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D100" s="3">
         <v>440</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="G100" s="5">
         <v>0.48</v>
@@ -9770,73 +9770,73 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -9844,7 +9844,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -9856,7 +9856,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G2" s="5">
         <v>0.1</v>
@@ -9912,10 +9912,10 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -9927,7 +9927,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G3" s="5">
         <v>0.125</v>
@@ -9983,10 +9983,10 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -9998,7 +9998,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G4" s="5">
         <v>0.15</v>
@@ -10054,10 +10054,10 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
@@ -10069,7 +10069,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G5" s="5">
         <v>0.18</v>
@@ -10125,10 +10125,10 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
@@ -10140,7 +10140,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G6" s="5">
         <v>0.2</v>
@@ -10196,10 +10196,10 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>2</v>
@@ -10211,7 +10211,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G7" s="5">
         <v>0.23</v>
@@ -10267,10 +10267,10 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2</v>
@@ -10282,7 +10282,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G8" s="5">
         <v>0.25</v>
@@ -10338,10 +10338,10 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
@@ -10353,7 +10353,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G9" s="5">
         <v>0.3</v>
@@ -10409,10 +10409,10 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -10424,7 +10424,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G10" s="5">
         <v>0.38</v>
@@ -10480,10 +10480,10 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
@@ -10495,7 +10495,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G11" s="5">
         <v>7.4999999999999997E-2</v>
@@ -10579,39 +10579,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" t="s">
         <v>145</v>
-      </c>
-      <c r="B1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
@@ -10625,16 +10625,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" s="10">
         <v>0.1</v>
@@ -10648,16 +10648,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
@@ -10671,16 +10671,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" s="10">
         <v>0.1</v>
@@ -10694,16 +10694,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E6" s="10">
         <v>0</v>
@@ -10717,16 +10717,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E7" s="10">
         <v>0.1</v>
@@ -10740,13 +10740,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D8">
         <v>250</v>
@@ -10763,13 +10763,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D9">
         <v>250</v>
@@ -10786,13 +10786,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D10">
         <v>250</v>
@@ -10809,13 +10809,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D11">
         <v>250</v>
@@ -10832,13 +10832,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D12">
         <v>250</v>
@@ -10855,13 +10855,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D13">
         <v>250</v>
@@ -10878,13 +10878,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D14">
         <v>250</v>
@@ -10901,13 +10901,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D15">
         <v>250</v>
@@ -10924,13 +10924,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D16">
         <v>250</v>
@@ -10947,13 +10947,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D17">
         <v>250</v>
@@ -10970,13 +10970,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D18">
         <v>200</v>
@@ -10993,13 +10993,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D19">
         <v>200</v>
@@ -11016,13 +11016,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D20">
         <v>300</v>
@@ -11039,13 +11039,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D21">
         <v>300</v>
@@ -11062,13 +11062,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D22">
         <v>300</v>
@@ -11085,13 +11085,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D23">
         <v>300</v>
@@ -11108,13 +11108,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D24">
         <v>300</v>
@@ -11131,13 +11131,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D25">
         <v>300</v>
@@ -11154,13 +11154,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D26">
         <v>300</v>
@@ -11177,13 +11177,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D27">
         <v>300</v>
@@ -11200,13 +11200,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D28">
         <v>300</v>
@@ -11223,13 +11223,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D29">
         <v>300</v>
@@ -11246,13 +11246,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D30">
         <v>300</v>
@@ -11269,13 +11269,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D31">
         <v>300</v>
@@ -11292,13 +11292,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D32">
         <v>350</v>
@@ -11315,13 +11315,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D33">
         <v>350</v>
@@ -11338,13 +11338,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D34">
         <v>350</v>
@@ -11361,13 +11361,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D35">
         <v>350</v>
@@ -11384,13 +11384,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B36" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C36" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D36">
         <v>350</v>
@@ -11407,13 +11407,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D37">
         <v>350</v>
@@ -11430,13 +11430,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D38">
         <v>350</v>
@@ -11453,13 +11453,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B39" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D39">
         <v>350</v>
@@ -11476,13 +11476,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D40">
         <v>400</v>
@@ -11499,13 +11499,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C41" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D41">
         <v>400</v>
@@ -11522,13 +11522,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C42" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D42">
         <v>400</v>
@@ -11545,13 +11545,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D43">
         <v>400</v>
@@ -11568,13 +11568,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C44" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D44">
         <v>400</v>
@@ -11591,13 +11591,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D45">
         <v>400</v>
@@ -11614,13 +11614,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D46">
         <v>450</v>
@@ -11637,13 +11637,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D47">
         <v>450</v>
@@ -11660,13 +11660,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D48">
         <v>450</v>
@@ -11683,13 +11683,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D49">
         <v>450</v>
@@ -11706,13 +11706,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B50" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D50">
         <v>450</v>
@@ -11729,13 +11729,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D51">
         <v>450</v>
@@ -11752,13 +11752,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C52" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D52">
         <v>350</v>
@@ -11775,13 +11775,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B53" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C53" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D53">
         <v>350</v>
@@ -11798,13 +11798,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B54" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C54" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D54">
         <v>350</v>
@@ -11821,13 +11821,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B55" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D55">
         <v>350</v>
@@ -11844,13 +11844,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D56">
         <v>350</v>
@@ -11867,13 +11867,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B57" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D57">
         <v>350</v>
@@ -11890,13 +11890,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D58">
         <v>300</v>
@@ -11913,13 +11913,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C59" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D59">
         <v>300</v>
@@ -11936,13 +11936,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B60" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C60" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D60">
         <v>300</v>
@@ -11959,13 +11959,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D61">
         <v>300</v>
@@ -11982,13 +11982,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B62" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D62">
         <v>300</v>
@@ -12005,13 +12005,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C63" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D63">
         <v>300</v>

</xml_diff>

<commit_message>
added steel plate dataframes.
</commit_message>
<xml_diff>
--- a/data/steel_data.xlsx
+++ b/data/steel_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F678EBC6-C156-4D2A-8E38-F9A35D457728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3861A22-A503-411F-8B9B-136A80EA4ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
+    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
   </bookViews>
   <sheets>
     <sheet name="Is" sheetId="1" r:id="rId1"/>
     <sheet name="Cs" sheetId="2" r:id="rId2"/>
     <sheet name="grades" sheetId="3" r:id="rId3"/>
+    <sheet name="standard_plate" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="163">
   <si>
     <t>d</t>
   </si>
@@ -522,13 +523,16 @@
   </si>
   <si>
     <t>welded</t>
+  </si>
+  <si>
+    <t>thickness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="0.0&quot; kg / m&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00&quot; kg / m&quot;"/>
     <numFmt numFmtId="166" formatCode="0.000&quot; m&quot;"/>
@@ -537,6 +541,7 @@
     <numFmt numFmtId="169" formatCode="##0.00E+00&quot; m³&quot;"/>
     <numFmt numFmtId="170" formatCode="##0.00E+00&quot; m⁶&quot;"/>
     <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -585,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -598,11 +603,18 @@
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="59">
+    <dxf>
+      <numFmt numFmtId="173" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="171" formatCode="0.0"/>
     </dxf>
@@ -1919,9 +1931,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="3" xr9:uid="{8A27988E-247C-4FF5-8CF3-24D483E6BCB9}">
-      <tableStyleElement type="wholeTable" dxfId="56"/>
-      <tableStyleElement type="headerRow" dxfId="55"/>
-      <tableStyleElement type="secondRowStripe" dxfId="54"/>
+      <tableStyleElement type="wholeTable" dxfId="58"/>
+      <tableStyleElement type="headerRow" dxfId="57"/>
+      <tableStyleElement type="secondRowStripe" dxfId="56"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1942,67 +1954,67 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:X100" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:X100" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="A1:X100" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="51"/>
-    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="44"/>
-    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="43"/>
-    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="42"/>
-    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="45"/>
+    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="41">
       <calculatedColumnFormula>IF(Table2[[#This Row],[w_1]]="",Table2[[#This Row],[r_1]],Table2[[#This Row],[w_1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="38"/>
-    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="37"/>
-    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="36"/>
-    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="35"/>
-    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="34"/>
-    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="33"/>
-    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="32"/>
-    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="31"/>
-    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="30"/>
-    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="29"/>
-    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="28"/>
+    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="40"/>
+    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="39"/>
+    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="38"/>
+    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="37"/>
+    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="36"/>
+    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="35"/>
+    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="34"/>
+    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="33"/>
+    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="32"/>
+    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="31"/>
+    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:W11" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="16"/>
-    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="15"/>
-    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="14"/>
-    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="13"/>
-    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="12"/>
-    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="11"/>
-    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="10"/>
-    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="9"/>
-    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="8"/>
-    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="7"/>
-    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="6"/>
-    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="5"/>
-    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="4"/>
-    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="17"/>
+    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="16"/>
+    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="15"/>
+    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="14"/>
+    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="13"/>
+    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="12"/>
+    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="11"/>
+    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="10"/>
+    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="9"/>
+    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="8"/>
+    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="7"/>
+    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="6"/>
+    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2016,9 +2028,19 @@
     <tableColumn id="7" xr3:uid="{F4DBA019-F123-4B98-A615-C1C293EAF7F6}" name="current"/>
     <tableColumn id="6" xr3:uid="{49F22BD6-5E2F-4DCD-B8F2-753E49B729CD}" name="form"/>
     <tableColumn id="2" xr3:uid="{D21D031E-2102-48DD-8FDF-9B85CD1F2DC4}" name="grade"/>
-    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:A21" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{30D98F40-E00D-49DD-B117-7321D335A518}" name="thickness" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2323,7 +2345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DE0702-9028-4C23-A846-1BC90EE38588}">
   <dimension ref="A1:X100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -12032,4 +12054,130 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD09439-A02C-4923-AF45-028C99498051}">
+  <dimension ref="A1:A21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add standard weld size dataframes and method to get nearest weld size.
</commit_message>
<xml_diff>
--- a/data/steel_data.xlsx
+++ b/data/steel_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3861A22-A503-411F-8B9B-136A80EA4ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BD5D72-8057-48E7-8EBA-917F0ADA4B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
+    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
   </bookViews>
   <sheets>
     <sheet name="Is" sheetId="1" r:id="rId1"/>
     <sheet name="Cs" sheetId="2" r:id="rId2"/>
     <sheet name="grades" sheetId="3" r:id="rId3"/>
     <sheet name="standard_plate" sheetId="4" r:id="rId4"/>
+    <sheet name="standard_fillet_welds" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="164">
   <si>
     <t>d</t>
   </si>
@@ -526,6 +527,9 @@
   </si>
   <si>
     <t>thickness</t>
+  </si>
+  <si>
+    <t>leg_size</t>
   </si>
 </sst>
 </file>
@@ -541,7 +545,7 @@
     <numFmt numFmtId="169" formatCode="##0.00E+00&quot; m³&quot;"/>
     <numFmt numFmtId="170" formatCode="##0.00E+00&quot; m⁶&quot;"/>
     <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -603,17 +607,23 @@
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="61">
     <dxf>
-      <numFmt numFmtId="173" formatCode="0.000"/>
+      <numFmt numFmtId="172" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="173" formatCode="0.000"/>
+      <numFmt numFmtId="172" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="171" formatCode="0.0"/>
@@ -1931,9 +1941,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="3" xr9:uid="{8A27988E-247C-4FF5-8CF3-24D483E6BCB9}">
-      <tableStyleElement type="wholeTable" dxfId="58"/>
-      <tableStyleElement type="headerRow" dxfId="57"/>
-      <tableStyleElement type="secondRowStripe" dxfId="56"/>
+      <tableStyleElement type="wholeTable" dxfId="60"/>
+      <tableStyleElement type="headerRow" dxfId="59"/>
+      <tableStyleElement type="secondRowStripe" dxfId="58"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1954,67 +1964,67 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:X100" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:X100" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="A1:X100" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="46"/>
-    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="45"/>
-    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="44"/>
-    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="41">
+    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="48"/>
+    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="47"/>
+    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="46"/>
+    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="43">
       <calculatedColumnFormula>IF(Table2[[#This Row],[w_1]]="",Table2[[#This Row],[r_1]],Table2[[#This Row],[w_1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="40"/>
-    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="39"/>
-    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="38"/>
-    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="37"/>
-    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="36"/>
-    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="35"/>
-    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="34"/>
-    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="33"/>
-    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="32"/>
-    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="31"/>
-    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="30"/>
+    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="42"/>
+    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="41"/>
+    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="40"/>
+    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="39"/>
+    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="38"/>
+    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="37"/>
+    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="36"/>
+    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="35"/>
+    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="34"/>
+    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="33"/>
+    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:W11" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="17"/>
-    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="16"/>
-    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="15"/>
-    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="14"/>
-    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="13"/>
-    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="12"/>
-    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="11"/>
-    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="10"/>
-    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="9"/>
-    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="8"/>
-    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="7"/>
-    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="6"/>
-    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="19"/>
+    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="18"/>
+    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="17"/>
+    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="16"/>
+    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="15"/>
+    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="14"/>
+    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="13"/>
+    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="12"/>
+    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="11"/>
+    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="10"/>
+    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="9"/>
+    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="8"/>
+    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2028,19 +2038,29 @@
     <tableColumn id="7" xr3:uid="{F4DBA019-F123-4B98-A615-C1C293EAF7F6}" name="current"/>
     <tableColumn id="6" xr3:uid="{49F22BD6-5E2F-4DCD-B8F2-753E49B729CD}" name="form"/>
     <tableColumn id="2" xr3:uid="{D21D031E-2102-48DD-8FDF-9B85CD1F2DC4}" name="grade"/>
-    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="A1:A21" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{30D98F40-E00D-49DD-B117-7321D335A518}" name="thickness" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{30D98F40-E00D-49DD-B117-7321D335A518}" name="thickness" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}" name="Table5" displayName="Table5" ref="A1:A10" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="A1:A10" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{3CB5E7CA-7DA9-4A14-81EC-A5B9BB9E0DFB}" name="leg_size" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12060,7 +12080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD09439-A02C-4923-AF45-028C99498051}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
@@ -12180,4 +12200,75 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19D2504-39AA-477C-A873-73FAEE5DD287}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bugs in angle_section_df_units.
</commit_message>
<xml_diff>
--- a/data/steel_data.xlsx
+++ b/data/steel_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E342BD-7B4B-41D7-AA73-62640492BF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55540A7A-3828-4DD4-98C4-44211D38F4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
   </bookViews>
@@ -36,28 +36,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11933,10 +11911,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CD5C03-AF5D-466E-B73D-7C4A1F62B2CE}">
-  <dimension ref="A1:AX66"/>
+  <dimension ref="A1:AU66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1:AX1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11975,7 +11953,7 @@
     <col min="47" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>119</v>
       </c>
@@ -12117,12 +12095,8 @@
       <c r="AU1" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="AX1" t="str" cm="1">
-        <f t="array" ref="AX1:AX47">TRANSPOSE(Table12[#Headers])</f>
-        <v>section</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>166</v>
       </c>
@@ -12264,11 +12238,8 @@
       <c r="AU2" s="20">
         <v>-4.4500000000000001E-9</v>
       </c>
-      <c r="AX2" t="str">
-        <v>current</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>165</v>
       </c>
@@ -12410,11 +12381,8 @@
       <c r="AU3" s="20">
         <v>-6.3199999999999997E-9</v>
       </c>
-      <c r="AX3" t="str">
-        <v>designation</v>
-      </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>164</v>
       </c>
@@ -12556,11 +12524,8 @@
       <c r="AU4" s="20">
         <v>-7.4999999999999993E-9</v>
       </c>
-      <c r="AX4" t="str">
-        <v>mass</v>
-      </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>169</v>
       </c>
@@ -12702,11 +12667,8 @@
       <c r="AU5" s="20">
         <v>-8.0399999999999995E-9</v>
       </c>
-      <c r="AX5" t="str">
-        <v>section_shape</v>
-      </c>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>168</v>
       </c>
@@ -12848,11 +12810,8 @@
       <c r="AU6" s="20">
         <v>-1.16E-8</v>
       </c>
-      <c r="AX6" t="str">
-        <v>fabrication_type</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>167</v>
       </c>
@@ -12994,11 +12953,8 @@
       <c r="AU7" s="20">
         <v>-1.4E-8</v>
       </c>
-      <c r="AX7" t="str">
-        <v>b_1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>172</v>
       </c>
@@ -13140,11 +13096,8 @@
       <c r="AU8" s="20">
         <v>-2.0100000000000001E-8</v>
       </c>
-      <c r="AX8" t="str">
-        <v>b_2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>171</v>
       </c>
@@ -13286,11 +13239,8 @@
       <c r="AU9" s="20">
         <v>-2.96E-8</v>
       </c>
-      <c r="AX9" t="str">
-        <v>t</v>
-      </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>170</v>
       </c>
@@ -13432,11 +13382,8 @@
       <c r="AU10" s="20">
         <v>-3.6599999999999997E-8</v>
       </c>
-      <c r="AX10" t="str">
-        <v>r_1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>175</v>
       </c>
@@ -13578,11 +13525,8 @@
       <c r="AU11" s="20">
         <v>-2.92E-8</v>
       </c>
-      <c r="AX11" t="str">
-        <v>r_2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>174</v>
       </c>
@@ -13724,11 +13668,8 @@
       <c r="AU12" s="20">
         <v>-4.3100000000000002E-8</v>
       </c>
-      <c r="AX12" t="str">
-        <v>a_g</v>
-      </c>
-    </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>173</v>
       </c>
@@ -13870,11 +13811,8 @@
       <c r="AU13" s="20">
         <v>-5.3799999999999999E-8</v>
       </c>
-      <c r="AX13" t="str">
-        <v>n_l</v>
-      </c>
-    </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>179</v>
       </c>
@@ -14016,11 +13954,8 @@
       <c r="AU14" s="20">
         <v>-4.0499999999999999E-8</v>
       </c>
-      <c r="AX14" t="str">
-        <v>n_r</v>
-      </c>
-    </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>178</v>
       </c>
@@ -14162,11 +14097,8 @@
       <c r="AU15" s="20">
         <v>-6.0199999999999996E-8</v>
       </c>
-      <c r="AX15" t="str">
-        <v>p_b</v>
-      </c>
-    </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>177</v>
       </c>
@@ -14308,11 +14240,8 @@
       <c r="AU16" s="20">
         <v>-7.5600000000000002E-8</v>
       </c>
-      <c r="AX16" t="str">
-        <v>p_t</v>
-      </c>
-    </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>176</v>
       </c>
@@ -14454,11 +14383,8 @@
       <c r="AU17" s="20">
         <v>-9.2799999999999997E-8</v>
       </c>
-      <c r="AX17" t="str">
-        <v>i_x</v>
-      </c>
-    </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>181</v>
       </c>
@@ -14600,11 +14526,8 @@
       <c r="AU18" s="20">
         <v>-8.1400000000000001E-8</v>
       </c>
-      <c r="AX18" t="str">
-        <v>y_1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>180</v>
       </c>
@@ -14746,11 +14669,8 @@
       <c r="AU19" s="20">
         <v>-1.03E-7</v>
       </c>
-      <c r="AX19" t="str">
-        <v>z_x1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>185</v>
       </c>
@@ -14892,11 +14812,8 @@
       <c r="AU20" s="20">
         <v>-1.3799999999999999E-7</v>
       </c>
-      <c r="AX20" t="str">
-        <v>y_4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>184</v>
       </c>
@@ -15038,11 +14955,8 @@
       <c r="AU21" s="20">
         <v>-1.7499999999999999E-7</v>
       </c>
-      <c r="AX21" t="str">
-        <v>z_x4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>183</v>
       </c>
@@ -15184,11 +15098,8 @@
       <c r="AU22" s="20">
         <v>-2.1799999999999999E-7</v>
       </c>
-      <c r="AX22" t="str">
-        <v>y_5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>182</v>
       </c>
@@ -15330,11 +15241,8 @@
       <c r="AU23" s="20">
         <v>-2.5400000000000002E-7</v>
       </c>
-      <c r="AX23" t="str">
-        <v>z_x5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>189</v>
       </c>
@@ -15476,11 +15384,8 @@
       <c r="AU24" s="20">
         <v>-2.0800000000000001E-7</v>
       </c>
-      <c r="AX24" t="str">
-        <v>s_x</v>
-      </c>
-    </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>188</v>
       </c>
@@ -15622,11 +15527,8 @@
       <c r="AU25" s="20">
         <v>-2.6800000000000002E-7</v>
       </c>
-      <c r="AX25" t="str">
-        <v>r_x</v>
-      </c>
-    </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>187</v>
       </c>
@@ -15768,11 +15670,8 @@
       <c r="AU26" s="20">
         <v>-3.3799999999999998E-7</v>
       </c>
-      <c r="AX26" t="str">
-        <v>i_y</v>
-      </c>
-    </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>186</v>
       </c>
@@ -15914,11 +15813,8 @@
       <c r="AU27" s="20">
         <v>-3.9900000000000001E-7</v>
       </c>
-      <c r="AX27" t="str">
-        <v>x_5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>192</v>
       </c>
@@ -16060,11 +15956,8 @@
       <c r="AU28" s="20">
         <v>-4.75E-7</v>
       </c>
-      <c r="AX28" t="str">
-        <v>z_y5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>191</v>
       </c>
@@ -16206,11 +16099,8 @@
       <c r="AU29" s="20">
         <v>-6.0399999999999996E-7</v>
       </c>
-      <c r="AX29" t="str">
-        <v>x_3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>190</v>
       </c>
@@ -16352,11 +16242,8 @@
       <c r="AU30" s="20">
         <v>-7.1600000000000001E-7</v>
       </c>
-      <c r="AX30" t="str">
-        <v>z_y3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>196</v>
       </c>
@@ -16498,11 +16385,8 @@
       <c r="AU31" s="20">
         <v>-6.61E-7</v>
       </c>
-      <c r="AX31" t="str">
-        <v>x_2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>195</v>
       </c>
@@ -16644,11 +16528,8 @@
       <c r="AU32" s="20">
         <v>-8.4200000000000005E-7</v>
       </c>
-      <c r="AX32" t="str">
-        <v>z_y2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>194</v>
       </c>
@@ -16790,11 +16671,8 @@
       <c r="AU33" s="20">
         <v>-9.9999999999999995E-7</v>
       </c>
-      <c r="AX33" t="str">
-        <v>s_y</v>
-      </c>
-    </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>193</v>
       </c>
@@ -16936,11 +16814,8 @@
       <c r="AU34" s="20">
         <v>-1.22E-6</v>
       </c>
-      <c r="AX34" t="str">
-        <v>r_y</v>
-      </c>
-    </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>200</v>
       </c>
@@ -17082,11 +16957,8 @@
       <c r="AU35" s="20">
         <v>-1.6899999999999999E-6</v>
       </c>
-      <c r="AX35" t="str">
-        <v>j</v>
-      </c>
-    </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>199</v>
       </c>
@@ -17228,11 +17100,8 @@
       <c r="AU36" s="20">
         <v>-2.0200000000000001E-6</v>
       </c>
-      <c r="AX36" t="str">
-        <v>tan_α</v>
-      </c>
-    </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>198</v>
       </c>
@@ -17374,11 +17243,8 @@
       <c r="AU37" s="20">
         <v>-2.48E-6</v>
       </c>
-      <c r="AX37" t="str">
-        <v>i_n</v>
-      </c>
-    </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>197</v>
       </c>
@@ -17520,11 +17386,8 @@
       <c r="AU38" s="20">
         <v>-3.1099999999999999E-6</v>
       </c>
-      <c r="AX38" t="str">
-        <v>z_nb</v>
-      </c>
-    </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>204</v>
       </c>
@@ -17666,11 +17529,8 @@
       <c r="AU39" s="20">
         <v>-3.5599999999999998E-6</v>
       </c>
-      <c r="AX39" t="str">
-        <v>z_nt</v>
-      </c>
-    </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>203</v>
       </c>
@@ -17812,11 +17672,8 @@
       <c r="AU40" s="20">
         <v>-4.4000000000000002E-6</v>
       </c>
-      <c r="AX40" t="str">
-        <v>s_n</v>
-      </c>
-    </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>202</v>
       </c>
@@ -17958,11 +17815,8 @@
       <c r="AU41" s="20">
         <v>-5.5799999999999999E-6</v>
       </c>
-      <c r="AX41" t="str">
-        <v>r_n</v>
-      </c>
-    </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>201</v>
       </c>
@@ -18104,11 +17958,8 @@
       <c r="AU42" s="20">
         <v>-6.4799999999999998E-6</v>
       </c>
-      <c r="AX42" t="str">
-        <v>i_p</v>
-      </c>
-    </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>209</v>
       </c>
@@ -18250,11 +18101,8 @@
       <c r="AU43" s="20">
         <v>-1.1600000000000001E-5</v>
       </c>
-      <c r="AX43" t="str">
-        <v>z_pl</v>
-      </c>
-    </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>208</v>
       </c>
@@ -18396,11 +18244,8 @@
       <c r="AU44" s="20">
         <v>-1.4E-5</v>
       </c>
-      <c r="AX44" t="str">
-        <v>z_pr</v>
-      </c>
-    </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>207</v>
       </c>
@@ -18542,11 +18387,8 @@
       <c r="AU45" s="20">
         <v>-1.5500000000000001E-5</v>
       </c>
-      <c r="AX45" t="str">
-        <v>s_p</v>
-      </c>
-    </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>206</v>
       </c>
@@ -18688,11 +18530,8 @@
       <c r="AU46" s="20">
         <v>-1.6900000000000001E-5</v>
       </c>
-      <c r="AX46" t="str">
-        <v>r_p</v>
-      </c>
-    </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>205</v>
       </c>
@@ -18834,11 +18673,8 @@
       <c r="AU47" s="20">
         <v>-2.09E-5</v>
       </c>
-      <c r="AX47" t="str">
-        <v>i_np</v>
-      </c>
-    </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
         <v>232</v>
       </c>

</xml_diff>

<commit_message>
add CHS sections into steel.py
</commit_message>
<xml_diff>
--- a/data/steel_data.xlsx
+++ b/data/steel_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACD0FCD-0938-4080-93D6-2D18941D1FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1358F105-7015-44C3-B3A0-CD2FD7225DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="1" r:id="rId1"/>
@@ -1606,9 +1606,6 @@
     <t>Cold Formed</t>
   </si>
   <si>
-    <t>section_type</t>
-  </si>
-  <si>
     <t>i</t>
   </si>
   <si>
@@ -1625,6 +1622,9 @@
   </si>
   <si>
     <t>AS/NZS1163:C350</t>
+  </si>
+  <si>
+    <t>AS/NZS1163:C250</t>
   </si>
 </sst>
 </file>
@@ -1891,28 +1891,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1921,166 +1921,25 @@
   </cellStyles>
   <dxfs count="161">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF404041"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="173" formatCode="0&quot; kg / m&quot;"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF404041"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF404041"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="172" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF404041"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="173" formatCode="0&quot; kg / m&quot;"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF404041"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF404041"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="172" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF404041"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF404041"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF404041"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF404041"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF404041"/>
-        </bottom>
-      </border>
+      <numFmt numFmtId="172" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF404041"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF404041"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF404041"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF404041"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF404041"/>
-        </bottom>
-      </border>
+      <numFmt numFmtId="172" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="171" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -2319,6 +2178,82 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="9"/>
+        <color rgb="FF404041"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF404041"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF404041"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF404041"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF404041"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF404041"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF404041"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF404041"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF404041"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF404041"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -2477,6 +2412,47 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF404041"/>
+        </left>
+        <top style="thin">
+          <color rgb="FF404041"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF404041"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2509,86 +2485,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF404041"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF404041"/>
-        </left>
-        <top style="thin">
-          <color rgb="FF404041"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF0F0F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF404041"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF404041"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FF404041"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF404041"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF404041"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF404041"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF404041"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF404041"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -3087,6 +2983,68 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF404041"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="173" formatCode="0&quot; kg / m&quot;"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF404041"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF404041"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF404041"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="173" formatCode="0&quot; kg / m&quot;"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF404041"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF404041"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -5565,6 +5523,48 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF404041"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF404041"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF404041"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF404041"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF404041"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF404041"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF404041"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF404041"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF0F0F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -5606,9 +5606,9 @@
       <tableStyleElement type="secondRowStripe" dxfId="158"/>
     </tableStyle>
     <tableStyle name="tblIntegral" pivot="0" count="3" xr9:uid="{4821CFE2-E7BC-41B3-BEAB-DCD62782FF50}">
-      <tableStyleElement type="wholeTable" dxfId="25"/>
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="secondRowStripe" dxfId="23"/>
+      <tableStyleElement type="wholeTable" dxfId="157"/>
+      <tableStyleElement type="headerRow" dxfId="156"/>
+      <tableStyleElement type="secondRowStripe" dxfId="155"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -5684,6 +5684,7 @@
       <sheetName val="UAdesSI"/>
       <sheetName val="UAdes"/>
       <sheetName val="lookups"/>
+      <sheetName val="Australian Standard Section Pro"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -5734,196 +5735,197 @@
       <sheetData sheetId="45"/>
       <sheetData sheetId="46"/>
       <sheetData sheetId="47"/>
+      <sheetData sheetId="48" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:X100" totalsRowShown="0" headerRowDxfId="157" dataDxfId="156">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:X100" totalsRowShown="0" headerRowDxfId="154" dataDxfId="153">
   <autoFilter ref="A1:X100" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="155"/>
-    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="154"/>
-    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="153"/>
-    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="152"/>
-    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="151"/>
-    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="150"/>
-    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="149"/>
-    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="148"/>
-    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="147"/>
-    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="146"/>
-    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="145"/>
-    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="144"/>
-    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="143">
+    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="152"/>
+    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="151"/>
+    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="150"/>
+    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="149"/>
+    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="148"/>
+    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="147"/>
+    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="146"/>
+    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="145"/>
+    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="144"/>
+    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="143"/>
+    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="142"/>
+    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="140">
       <calculatedColumnFormula>IF(Table2[[#This Row],[w_1]]="",Table2[[#This Row],[r_1]],Table2[[#This Row],[w_1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="142"/>
-    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="141"/>
-    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="140"/>
-    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="139"/>
-    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="138"/>
-    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="137"/>
-    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="136"/>
-    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="135"/>
-    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="134"/>
-    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="133"/>
-    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="132"/>
+    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="139"/>
+    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="138"/>
+    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="137"/>
+    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="136"/>
+    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="135"/>
+    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="134"/>
+    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="133"/>
+    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="132"/>
+    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="131"/>
+    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="130"/>
+    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
   <autoFilter ref="A1:W11" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="129"/>
-    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="128"/>
-    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="126"/>
-    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="125"/>
-    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="124"/>
-    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="123"/>
-    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="122"/>
-    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="121"/>
-    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="120"/>
-    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="119"/>
-    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="118"/>
-    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="117"/>
-    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="116"/>
-    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="115"/>
-    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="114"/>
-    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="113"/>
-    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="112"/>
-    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="111"/>
-    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="110"/>
-    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="109"/>
-    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="108"/>
-    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="107"/>
+    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="126"/>
+    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="122"/>
+    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="121"/>
+    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="120"/>
+    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="119"/>
+    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="118"/>
+    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="117"/>
+    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="116"/>
+    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="115"/>
+    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="114"/>
+    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="113"/>
+    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="112"/>
+    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="111"/>
+    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="110"/>
+    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="109"/>
+    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="108"/>
+    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="107"/>
+    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="106"/>
+    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="105"/>
+    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{FF45E8D3-7736-40A7-99D3-559A453C579A}" name="Table12" displayName="Table12" ref="A1:AU66" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{FF45E8D3-7736-40A7-99D3-559A453C579A}" name="Table12" displayName="Table12" ref="A1:AU66" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
   <autoFilter ref="A1:AU66" xr:uid="{FF45E8D3-7736-40A7-99D3-559A453C579A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AU66">
     <sortCondition ref="E1:E66"/>
   </sortState>
   <tableColumns count="47">
-    <tableColumn id="1" xr3:uid="{0E98BFEB-C2F6-42CB-BF8F-C98E1C2E0635}" name="section" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{F8D7BC1B-0DBB-4D99-A300-0E4A90580804}" name="current" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{737CBCED-510B-4F43-B438-2A185FDD6050}" name="designation" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{B458591C-C4BC-4B79-957E-957A01651592}" name="mass" dataDxfId="101"/>
-    <tableColumn id="5" xr3:uid="{1795098C-FBE6-4A95-BF2C-C1D46892588F}" name="section_shape" dataDxfId="100"/>
-    <tableColumn id="6" xr3:uid="{A5CADDBA-1B4B-4115-9488-87017E29615A}" name="fabrication_type" dataDxfId="99"/>
-    <tableColumn id="7" xr3:uid="{238018DD-1F33-4BFE-A2AF-9CECCB06C3F0}" name="b_1" dataDxfId="98"/>
-    <tableColumn id="8" xr3:uid="{9D65AF38-BBE8-40A0-8C16-DFFFAF6CE138}" name="b_2" dataDxfId="97"/>
-    <tableColumn id="9" xr3:uid="{C2203BF0-6699-4823-92F5-390D9CF47F55}" name="t" dataDxfId="96"/>
-    <tableColumn id="10" xr3:uid="{FA82C60C-E6CB-4F75-8515-D3578B68A869}" name="r_1" dataDxfId="95"/>
-    <tableColumn id="11" xr3:uid="{98A4E8DE-21C5-4253-BB88-17B4789DF415}" name="r_2" dataDxfId="94"/>
-    <tableColumn id="14" xr3:uid="{89C8E045-1AD0-433A-B56D-64CF79A5DB3B}" name="a_g" dataDxfId="93"/>
-    <tableColumn id="15" xr3:uid="{0D147C1F-E2B1-4610-8F7F-2F2EDE479941}" name="n_l" dataDxfId="92"/>
-    <tableColumn id="16" xr3:uid="{7837E9B6-E904-4A0F-9F43-CD9FAA135778}" name="n_r" dataDxfId="91"/>
-    <tableColumn id="17" xr3:uid="{F2DB37C1-C66D-4D2D-A8C4-CCCC0ABE5FD7}" name="p_b" dataDxfId="90"/>
-    <tableColumn id="18" xr3:uid="{C3A966E4-6303-4391-9FEA-B96F8F3AB726}" name="p_t" dataDxfId="89"/>
-    <tableColumn id="19" xr3:uid="{06E33A70-92D2-4F18-AECA-57AB30FEB440}" name="i_x" dataDxfId="88"/>
-    <tableColumn id="20" xr3:uid="{9AA65A25-E661-4FAA-AF1D-3D44249D01BF}" name="y_1" dataDxfId="87"/>
-    <tableColumn id="21" xr3:uid="{9A701A27-0B2D-4F45-81BA-39175FEAF0B6}" name="z_x1" dataDxfId="86"/>
-    <tableColumn id="22" xr3:uid="{393FFFA1-B351-4FB1-9277-D50B0910FC0F}" name="y_4" dataDxfId="85"/>
-    <tableColumn id="23" xr3:uid="{2DACC83C-2104-45C1-B9FE-49A63E6E85E4}" name="z_x4" dataDxfId="84"/>
-    <tableColumn id="24" xr3:uid="{5D3F7ABB-7C07-476D-8F2A-742862304A6F}" name="y_5" dataDxfId="83"/>
-    <tableColumn id="25" xr3:uid="{A99B6213-CC3A-4218-A472-E5962B98B458}" name="z_x5" dataDxfId="82"/>
-    <tableColumn id="26" xr3:uid="{75554A80-CD5A-41AC-B6C7-07931FBCB5CB}" name="s_x" dataDxfId="81"/>
-    <tableColumn id="27" xr3:uid="{1C7FD4BF-A120-42D4-9F49-D421ACED02E5}" name="r_x" dataDxfId="80"/>
-    <tableColumn id="28" xr3:uid="{C0B7DB03-B03F-402C-B521-F68B9E6DCB6B}" name="i_y" dataDxfId="79"/>
-    <tableColumn id="29" xr3:uid="{E115797B-BC29-4A13-A6FE-C3C97DFB7135}" name="x_5" dataDxfId="78"/>
-    <tableColumn id="30" xr3:uid="{9E6BF5E6-1873-4844-80B3-E26FC413F5F2}" name="z_y5" dataDxfId="77"/>
-    <tableColumn id="31" xr3:uid="{C645FD7B-D220-4837-8F91-44B3ECD3B912}" name="x_3" dataDxfId="76"/>
-    <tableColumn id="32" xr3:uid="{778B9CFC-50E3-42F0-BF16-6835B2AA19C1}" name="z_y3" dataDxfId="75"/>
-    <tableColumn id="33" xr3:uid="{EE964793-FB8A-4B7C-8D5C-91F411165876}" name="x_2" dataDxfId="74"/>
-    <tableColumn id="34" xr3:uid="{3FE64EFF-34A4-413C-BB0F-062966F896E8}" name="z_y2" dataDxfId="73"/>
-    <tableColumn id="35" xr3:uid="{51D846ED-D7C5-4402-99F2-0DB0F2C24DD3}" name="s_y" dataDxfId="72"/>
-    <tableColumn id="36" xr3:uid="{E2B67361-9A2E-4480-B277-5C2ECFFB818C}" name="r_y" dataDxfId="71"/>
-    <tableColumn id="37" xr3:uid="{F2242E23-7412-4D7B-ACEB-6A0702AD99FA}" name="j" dataDxfId="70"/>
-    <tableColumn id="38" xr3:uid="{1FDDA5D1-FC4C-4923-B73E-C3BC38E38DB6}" name="tan_alpha" dataDxfId="69"/>
-    <tableColumn id="40" xr3:uid="{28747A12-AFEB-4090-B870-6FD912461659}" name="i_n" dataDxfId="68"/>
-    <tableColumn id="41" xr3:uid="{ED8FF4DA-2F9F-4152-8C5A-8E0D76DCA0E5}" name="z_nb" dataDxfId="67"/>
-    <tableColumn id="42" xr3:uid="{3DAA48FF-3532-4FE6-9832-4F6220A62A72}" name="z_nt" dataDxfId="66"/>
-    <tableColumn id="43" xr3:uid="{833FEA35-FCDE-463A-9087-A72AF4E331D5}" name="s_n" dataDxfId="65"/>
-    <tableColumn id="44" xr3:uid="{76B26717-A708-41FD-B8BD-EDA04EF167FC}" name="r_n" dataDxfId="64"/>
-    <tableColumn id="45" xr3:uid="{0B580395-0F1E-4B42-B46E-986CC167FEB3}" name="i_p" dataDxfId="63"/>
-    <tableColumn id="46" xr3:uid="{B9B6BEC6-FD25-41F9-892E-85B8845293E8}" name="z_pl" dataDxfId="62"/>
-    <tableColumn id="47" xr3:uid="{BE8BC5FB-D341-475B-942A-9E50AAA5F9C0}" name="z_pr" dataDxfId="61"/>
-    <tableColumn id="48" xr3:uid="{5BC5C573-CC69-4C9D-9ADE-BA3B1527D7A6}" name="s_p" dataDxfId="60"/>
-    <tableColumn id="49" xr3:uid="{9463694C-A3D5-479B-9FFE-37EE8D4FB591}" name="r_p" dataDxfId="59"/>
-    <tableColumn id="50" xr3:uid="{95621574-0C57-4E53-9BC0-FC033C0A02B9}" name="i_np" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{0E98BFEB-C2F6-42CB-BF8F-C98E1C2E0635}" name="section" dataDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{F8D7BC1B-0DBB-4D99-A300-0E4A90580804}" name="current" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{737CBCED-510B-4F43-B438-2A185FDD6050}" name="designation" dataDxfId="99"/>
+    <tableColumn id="4" xr3:uid="{B458591C-C4BC-4B79-957E-957A01651592}" name="mass" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{1795098C-FBE6-4A95-BF2C-C1D46892588F}" name="section_shape" dataDxfId="97"/>
+    <tableColumn id="6" xr3:uid="{A5CADDBA-1B4B-4115-9488-87017E29615A}" name="fabrication_type" dataDxfId="96"/>
+    <tableColumn id="7" xr3:uid="{238018DD-1F33-4BFE-A2AF-9CECCB06C3F0}" name="b_1" dataDxfId="95"/>
+    <tableColumn id="8" xr3:uid="{9D65AF38-BBE8-40A0-8C16-DFFFAF6CE138}" name="b_2" dataDxfId="94"/>
+    <tableColumn id="9" xr3:uid="{C2203BF0-6699-4823-92F5-390D9CF47F55}" name="t" dataDxfId="93"/>
+    <tableColumn id="10" xr3:uid="{FA82C60C-E6CB-4F75-8515-D3578B68A869}" name="r_1" dataDxfId="92"/>
+    <tableColumn id="11" xr3:uid="{98A4E8DE-21C5-4253-BB88-17B4789DF415}" name="r_2" dataDxfId="91"/>
+    <tableColumn id="14" xr3:uid="{89C8E045-1AD0-433A-B56D-64CF79A5DB3B}" name="a_g" dataDxfId="90"/>
+    <tableColumn id="15" xr3:uid="{0D147C1F-E2B1-4610-8F7F-2F2EDE479941}" name="n_l" dataDxfId="89"/>
+    <tableColumn id="16" xr3:uid="{7837E9B6-E904-4A0F-9F43-CD9FAA135778}" name="n_r" dataDxfId="88"/>
+    <tableColumn id="17" xr3:uid="{F2DB37C1-C66D-4D2D-A8C4-CCCC0ABE5FD7}" name="p_b" dataDxfId="87"/>
+    <tableColumn id="18" xr3:uid="{C3A966E4-6303-4391-9FEA-B96F8F3AB726}" name="p_t" dataDxfId="86"/>
+    <tableColumn id="19" xr3:uid="{06E33A70-92D2-4F18-AECA-57AB30FEB440}" name="i_x" dataDxfId="85"/>
+    <tableColumn id="20" xr3:uid="{9AA65A25-E661-4FAA-AF1D-3D44249D01BF}" name="y_1" dataDxfId="84"/>
+    <tableColumn id="21" xr3:uid="{9A701A27-0B2D-4F45-81BA-39175FEAF0B6}" name="z_x1" dataDxfId="83"/>
+    <tableColumn id="22" xr3:uid="{393FFFA1-B351-4FB1-9277-D50B0910FC0F}" name="y_4" dataDxfId="82"/>
+    <tableColumn id="23" xr3:uid="{2DACC83C-2104-45C1-B9FE-49A63E6E85E4}" name="z_x4" dataDxfId="81"/>
+    <tableColumn id="24" xr3:uid="{5D3F7ABB-7C07-476D-8F2A-742862304A6F}" name="y_5" dataDxfId="80"/>
+    <tableColumn id="25" xr3:uid="{A99B6213-CC3A-4218-A472-E5962B98B458}" name="z_x5" dataDxfId="79"/>
+    <tableColumn id="26" xr3:uid="{75554A80-CD5A-41AC-B6C7-07931FBCB5CB}" name="s_x" dataDxfId="78"/>
+    <tableColumn id="27" xr3:uid="{1C7FD4BF-A120-42D4-9F49-D421ACED02E5}" name="r_x" dataDxfId="77"/>
+    <tableColumn id="28" xr3:uid="{C0B7DB03-B03F-402C-B521-F68B9E6DCB6B}" name="i_y" dataDxfId="76"/>
+    <tableColumn id="29" xr3:uid="{E115797B-BC29-4A13-A6FE-C3C97DFB7135}" name="x_5" dataDxfId="75"/>
+    <tableColumn id="30" xr3:uid="{9E6BF5E6-1873-4844-80B3-E26FC413F5F2}" name="z_y5" dataDxfId="74"/>
+    <tableColumn id="31" xr3:uid="{C645FD7B-D220-4837-8F91-44B3ECD3B912}" name="x_3" dataDxfId="73"/>
+    <tableColumn id="32" xr3:uid="{778B9CFC-50E3-42F0-BF16-6835B2AA19C1}" name="z_y3" dataDxfId="72"/>
+    <tableColumn id="33" xr3:uid="{EE964793-FB8A-4B7C-8D5C-91F411165876}" name="x_2" dataDxfId="71"/>
+    <tableColumn id="34" xr3:uid="{3FE64EFF-34A4-413C-BB0F-062966F896E8}" name="z_y2" dataDxfId="70"/>
+    <tableColumn id="35" xr3:uid="{51D846ED-D7C5-4402-99F2-0DB0F2C24DD3}" name="s_y" dataDxfId="69"/>
+    <tableColumn id="36" xr3:uid="{E2B67361-9A2E-4480-B277-5C2ECFFB818C}" name="r_y" dataDxfId="68"/>
+    <tableColumn id="37" xr3:uid="{F2242E23-7412-4D7B-ACEB-6A0702AD99FA}" name="j" dataDxfId="67"/>
+    <tableColumn id="38" xr3:uid="{1FDDA5D1-FC4C-4923-B73E-C3BC38E38DB6}" name="tan_alpha" dataDxfId="66"/>
+    <tableColumn id="40" xr3:uid="{28747A12-AFEB-4090-B870-6FD912461659}" name="i_n" dataDxfId="65"/>
+    <tableColumn id="41" xr3:uid="{ED8FF4DA-2F9F-4152-8C5A-8E0D76DCA0E5}" name="z_nb" dataDxfId="64"/>
+    <tableColumn id="42" xr3:uid="{3DAA48FF-3532-4FE6-9832-4F6220A62A72}" name="z_nt" dataDxfId="63"/>
+    <tableColumn id="43" xr3:uid="{833FEA35-FCDE-463A-9087-A72AF4E331D5}" name="s_n" dataDxfId="62"/>
+    <tableColumn id="44" xr3:uid="{76B26717-A708-41FD-B8BD-EDA04EF167FC}" name="r_n" dataDxfId="61"/>
+    <tableColumn id="45" xr3:uid="{0B580395-0F1E-4B42-B46E-986CC167FEB3}" name="i_p" dataDxfId="60"/>
+    <tableColumn id="46" xr3:uid="{B9B6BEC6-FD25-41F9-892E-85B8845293E8}" name="z_pl" dataDxfId="59"/>
+    <tableColumn id="47" xr3:uid="{BE8BC5FB-D341-475B-942A-9E50AAA5F9C0}" name="z_pr" dataDxfId="58"/>
+    <tableColumn id="48" xr3:uid="{5BC5C573-CC69-4C9D-9ADE-BA3B1527D7A6}" name="s_p" dataDxfId="57"/>
+    <tableColumn id="49" xr3:uid="{9463694C-A3D5-479B-9FFE-37EE8D4FB591}" name="r_p" dataDxfId="56"/>
+    <tableColumn id="50" xr3:uid="{95621574-0C57-4E53-9BC0-FC033C0A02B9}" name="i_np" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F856F8D5-18F2-4A4D-B287-05A7E0FF4BE1}" name="Table6" displayName="Table6" ref="A1:W214" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F856F8D5-18F2-4A4D-B287-05A7E0FF4BE1}" name="Table6" displayName="Table6" ref="A1:W214" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51">
   <autoFilter ref="A1:W214" xr:uid="{F856F8D5-18F2-4A4D-B287-05A7E0FF4BE1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U5">
     <sortCondition ref="C1:C5"/>
   </sortState>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{E2925810-9C25-4132-BD5C-0C5A42D6A5EC}" name="section" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{29DF28F2-F045-4FB5-9C6A-137EF8CD95BE}" name="current" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{E0220977-C835-4F23-84EE-414C1FB0AAE1}" name="designation" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{4AD71210-471B-4703-AB9B-F486971BA2A1}" name="mass" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{DD9D9038-D97E-4758-8DD0-B14CA71C812F}" name="section_shape" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{02672C8D-03B0-4D8B-8619-4432D5969A4A}" name="fabrication_type" dataDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{4A188572-EC44-4443-9EC8-90B6ED8DA804}" name="grade" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{827373FC-F25E-4349-AD07-EAFEB6B115C2}" name="standard" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{3A7583DF-88D0-45A3-97CD-7706449B782E}" name="d" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{4AD1418E-6E9D-439F-8B4F-3B3CFA20B544}" name="b" dataDxfId="46"/>
-    <tableColumn id="13" xr3:uid="{287D0ED0-248B-4DD9-9BCD-A6EE331603B8}" name="t" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{1CC4C8E3-54B6-464C-A529-82FE3496DB64}" name="r_ext" dataDxfId="44"/>
-    <tableColumn id="16" xr3:uid="{77049593-28F1-4D83-8C14-F10F3E66A5D7}" name="a_g" dataDxfId="43"/>
-    <tableColumn id="17" xr3:uid="{3240AB16-E873-4A2B-B3DA-861D829AE31F}" name="i_x" dataDxfId="42"/>
-    <tableColumn id="18" xr3:uid="{8B09D638-0194-4AC0-BBD4-61DD2A62D3AB}" name="z_x" dataDxfId="41"/>
-    <tableColumn id="19" xr3:uid="{8E60B5AE-75F6-43E6-8862-AE98480D9A53}" name="s_x" dataDxfId="40"/>
-    <tableColumn id="20" xr3:uid="{14931501-0531-428B-B2FA-9C5C9B8D963D}" name="r_x" dataDxfId="39"/>
-    <tableColumn id="21" xr3:uid="{C394B290-F7E3-4AA0-AFC7-C2D2C979FDD1}" name="i_y" dataDxfId="38"/>
-    <tableColumn id="22" xr3:uid="{4E103565-1C69-4681-81A6-991D62E282C9}" name="z_y" dataDxfId="37"/>
-    <tableColumn id="23" xr3:uid="{B4451F83-E157-42F5-81A7-D27C6265A445}" name="s_y" dataDxfId="36"/>
-    <tableColumn id="24" xr3:uid="{C7B5BFBB-6023-44E8-9480-8F7249B60E9C}" name="r_y" dataDxfId="35"/>
-    <tableColumn id="27" xr3:uid="{121A9941-351F-4C3C-A65A-73C4C311794F}" name="j" dataDxfId="34"/>
-    <tableColumn id="28" xr3:uid="{88B2FE0E-4A60-40F1-8D6E-111D544F2617}" name="c" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{E2925810-9C25-4132-BD5C-0C5A42D6A5EC}" name="section" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{29DF28F2-F045-4FB5-9C6A-137EF8CD95BE}" name="current" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{E0220977-C835-4F23-84EE-414C1FB0AAE1}" name="designation" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{4AD71210-471B-4703-AB9B-F486971BA2A1}" name="mass" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{DD9D9038-D97E-4758-8DD0-B14CA71C812F}" name="section_shape" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{02672C8D-03B0-4D8B-8619-4432D5969A4A}" name="fabrication_type" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{4A188572-EC44-4443-9EC8-90B6ED8DA804}" name="grade" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{827373FC-F25E-4349-AD07-EAFEB6B115C2}" name="standard" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{3A7583DF-88D0-45A3-97CD-7706449B782E}" name="d" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{4AD1418E-6E9D-439F-8B4F-3B3CFA20B544}" name="b" dataDxfId="41"/>
+    <tableColumn id="13" xr3:uid="{287D0ED0-248B-4DD9-9BCD-A6EE331603B8}" name="t" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{1CC4C8E3-54B6-464C-A529-82FE3496DB64}" name="r_ext" dataDxfId="39"/>
+    <tableColumn id="16" xr3:uid="{77049593-28F1-4D83-8C14-F10F3E66A5D7}" name="a_g" dataDxfId="38"/>
+    <tableColumn id="17" xr3:uid="{3240AB16-E873-4A2B-B3DA-861D829AE31F}" name="i_x" dataDxfId="37"/>
+    <tableColumn id="18" xr3:uid="{8B09D638-0194-4AC0-BBD4-61DD2A62D3AB}" name="z_x" dataDxfId="36"/>
+    <tableColumn id="19" xr3:uid="{8E60B5AE-75F6-43E6-8862-AE98480D9A53}" name="s_x" dataDxfId="35"/>
+    <tableColumn id="20" xr3:uid="{14931501-0531-428B-B2FA-9C5C9B8D963D}" name="r_x" dataDxfId="34"/>
+    <tableColumn id="21" xr3:uid="{C394B290-F7E3-4AA0-AFC7-C2D2C979FDD1}" name="i_y" dataDxfId="33"/>
+    <tableColumn id="22" xr3:uid="{4E103565-1C69-4681-81A6-991D62E282C9}" name="z_y" dataDxfId="32"/>
+    <tableColumn id="23" xr3:uid="{B4451F83-E157-42F5-81A7-D27C6265A445}" name="s_y" dataDxfId="31"/>
+    <tableColumn id="24" xr3:uid="{C7B5BFBB-6023-44E8-9480-8F7249B60E9C}" name="r_y" dataDxfId="30"/>
+    <tableColumn id="27" xr3:uid="{121A9941-351F-4C3C-A65A-73C4C311794F}" name="j" dataDxfId="29"/>
+    <tableColumn id="28" xr3:uid="{88B2FE0E-4A60-40F1-8D6E-111D544F2617}" name="c" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{82015ECB-7CED-4ACD-A99C-225C1D660049}" name="Table9" displayName="Table9" ref="A1:Q74" totalsRowShown="0" headerRowDxfId="20" dataDxfId="4" headerRowBorderDxfId="21" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{82015ECB-7CED-4ACD-A99C-225C1D660049}" name="Table9" displayName="Table9" ref="A1:Q74" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24">
   <autoFilter ref="A1:Q74" xr:uid="{82015ECB-7CED-4ACD-A99C-225C1D660049}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q74">
     <sortCondition ref="G1:G74"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{F989E24A-2895-403A-95D8-FB6D57B33393}" name="section" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{3A3AA581-72B7-4C71-92ED-58FF0AF8C58F}" name="current" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{4AF474D4-D6CD-478F-9C12-9E3BD9498538}" name="designation" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{FB925A7C-C5BD-4C4F-B3B7-409904034742}" name="mass" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{671391B3-7819-4686-B553-6816137ABD4C}" name="section_type" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{D1A5F5F4-1AC1-4423-A8A6-FFF97CAE9132}" name="fabrication_type" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{370D76B4-ED4B-4369-B0DA-F466EE63D50C}" name="grade" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{7D379C42-B6F9-4886-BC19-6BB4717591C7}" name="standard" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{F287B4A8-95A8-4F80-AA3C-6CB66011704D}" name="d" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{9B5E365E-AF5E-4F63-8A33-962C2AB3671D}" name="t" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{85DE6BC4-7DB1-431E-9156-2965CE49DB00}" name="a_g" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{D2661048-444D-4C95-9F11-0677EC8A1982}" name="i" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{F0DAF1A3-96B3-492E-AFF5-13A74AD474B2}" name="z" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{905A8923-FED3-4886-87C3-EFFB3C0C84D5}" name="s" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{89747857-0C0B-4369-A11D-5A861AD3C77F}" name="r" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{6720023D-EA79-4ECC-BBC2-79CB176A6FA2}" name="j" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{792A3F36-2BD7-4DC0-9411-D3763E15297D}" name="c" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{F989E24A-2895-403A-95D8-FB6D57B33393}" name="section" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{3A3AA581-72B7-4C71-92ED-58FF0AF8C58F}" name="current" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{4AF474D4-D6CD-478F-9C12-9E3BD9498538}" name="designation" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{FB925A7C-C5BD-4C4F-B3B7-409904034742}" name="mass" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{671391B3-7819-4686-B553-6816137ABD4C}" name="section_shape" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{D1A5F5F4-1AC1-4423-A8A6-FFF97CAE9132}" name="fabrication_type" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{370D76B4-ED4B-4369-B0DA-F466EE63D50C}" name="grade" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{7D379C42-B6F9-4886-BC19-6BB4717591C7}" name="standard" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{F287B4A8-95A8-4F80-AA3C-6CB66011704D}" name="d" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{9B5E365E-AF5E-4F63-8A33-962C2AB3671D}" name="t" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{85DE6BC4-7DB1-431E-9156-2965CE49DB00}" name="a_g" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{D2661048-444D-4C95-9F11-0677EC8A1982}" name="i" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{F0DAF1A3-96B3-492E-AFF5-13A74AD474B2}" name="z" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{905A8923-FED3-4886-87C3-EFFB3C0C84D5}" name="s" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{89747857-0C0B-4369-A11D-5A861AD3C77F}" name="r" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{6720023D-EA79-4ECC-BBC2-79CB176A6FA2}" name="j" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{792A3F36-2BD7-4DC0-9411-D3763E15297D}" name="c" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5937,29 +5939,29 @@
     <tableColumn id="7" xr3:uid="{F4DBA019-F123-4B98-A615-C1C293EAF7F6}" name="current"/>
     <tableColumn id="6" xr3:uid="{49F22BD6-5E2F-4DCD-B8F2-753E49B729CD}" name="form"/>
     <tableColumn id="2" xr3:uid="{D21D031E-2102-48DD-8FDF-9B85CD1F2DC4}" name="grade"/>
-    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="A1:A21" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{30D98F40-E00D-49DD-B117-7321D335A518}" name="thickness" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{30D98F40-E00D-49DD-B117-7321D335A518}" name="thickness" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}" name="Table5" displayName="Table5" ref="A1:A11" totalsRowShown="0" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}" name="Table5" displayName="Table5" ref="A1:A11" totalsRowShown="0" dataDxfId="1">
   <autoFilter ref="A1:A11" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3CB5E7CA-7DA9-4A14-81EC-A5B9BB9E0DFB}" name="leg_size" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{3CB5E7CA-7DA9-4A14-81EC-A5B9BB9E0DFB}" name="leg_size" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -23990,8 +23992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41821909-ADF1-4A45-9D48-644384A7A2E3}">
   <dimension ref="A1:W214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24103,7 +24105,7 @@
         <v>349</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>143</v>
@@ -24174,7 +24176,7 @@
         <v>349</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H3" s="29" t="s">
         <v>143</v>
@@ -24245,7 +24247,7 @@
         <v>349</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H4" s="29" t="s">
         <v>143</v>
@@ -24316,7 +24318,7 @@
         <v>349</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H5" s="37" t="s">
         <v>143</v>
@@ -24387,7 +24389,7 @@
         <v>349</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H6" s="29" t="s">
         <v>143</v>
@@ -24458,7 +24460,7 @@
         <v>349</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H7" s="29" t="s">
         <v>143</v>
@@ -24529,7 +24531,7 @@
         <v>349</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H8" s="29" t="s">
         <v>143</v>
@@ -24600,7 +24602,7 @@
         <v>349</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H9" s="37" t="s">
         <v>143</v>
@@ -24671,7 +24673,7 @@
         <v>349</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H10" s="29" t="s">
         <v>143</v>
@@ -24742,7 +24744,7 @@
         <v>349</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H11" s="29" t="s">
         <v>143</v>
@@ -24813,7 +24815,7 @@
         <v>349</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>143</v>
@@ -24884,7 +24886,7 @@
         <v>349</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H13" s="37" t="s">
         <v>143</v>
@@ -24955,7 +24957,7 @@
         <v>349</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>143</v>
@@ -25026,7 +25028,7 @@
         <v>349</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H15" s="29" t="s">
         <v>143</v>
@@ -25097,7 +25099,7 @@
         <v>349</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H16" s="29" t="s">
         <v>143</v>
@@ -25168,7 +25170,7 @@
         <v>349</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H17" s="37" t="s">
         <v>143</v>
@@ -25239,7 +25241,7 @@
         <v>349</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H18" s="29" t="s">
         <v>143</v>
@@ -25310,7 +25312,7 @@
         <v>349</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H19" s="29" t="s">
         <v>143</v>
@@ -25381,7 +25383,7 @@
         <v>349</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H20" s="29" t="s">
         <v>143</v>
@@ -25452,7 +25454,7 @@
         <v>349</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H21" s="37" t="s">
         <v>143</v>
@@ -25523,7 +25525,7 @@
         <v>349</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H22" s="29" t="s">
         <v>143</v>
@@ -25594,7 +25596,7 @@
         <v>349</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H23" s="29" t="s">
         <v>143</v>
@@ -25665,7 +25667,7 @@
         <v>349</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>143</v>
@@ -25736,7 +25738,7 @@
         <v>349</v>
       </c>
       <c r="G25" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H25" s="37" t="s">
         <v>143</v>
@@ -25807,7 +25809,7 @@
         <v>349</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H26" s="29" t="s">
         <v>143</v>
@@ -25878,7 +25880,7 @@
         <v>349</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>143</v>
@@ -25949,7 +25951,7 @@
         <v>349</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>143</v>
@@ -26020,7 +26022,7 @@
         <v>349</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H29" s="37" t="s">
         <v>143</v>
@@ -26091,7 +26093,7 @@
         <v>349</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H30" s="29" t="s">
         <v>143</v>
@@ -26162,7 +26164,7 @@
         <v>349</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H31" s="29" t="s">
         <v>143</v>
@@ -26233,7 +26235,7 @@
         <v>349</v>
       </c>
       <c r="G32" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H32" s="29" t="s">
         <v>143</v>
@@ -26304,7 +26306,7 @@
         <v>349</v>
       </c>
       <c r="G33" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H33" s="37" t="s">
         <v>143</v>
@@ -26375,7 +26377,7 @@
         <v>349</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H34" s="29" t="s">
         <v>143</v>
@@ -26446,7 +26448,7 @@
         <v>349</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H35" s="29" t="s">
         <v>143</v>
@@ -26517,7 +26519,7 @@
         <v>349</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H36" s="29" t="s">
         <v>143</v>
@@ -26588,7 +26590,7 @@
         <v>349</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H37" s="37" t="s">
         <v>143</v>
@@ -26659,7 +26661,7 @@
         <v>349</v>
       </c>
       <c r="G38" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H38" s="29" t="s">
         <v>143</v>
@@ -26730,7 +26732,7 @@
         <v>349</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H39" s="29" t="s">
         <v>143</v>
@@ -26801,7 +26803,7 @@
         <v>349</v>
       </c>
       <c r="G40" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H40" s="29" t="s">
         <v>143</v>
@@ -26872,7 +26874,7 @@
         <v>349</v>
       </c>
       <c r="G41" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H41" s="37" t="s">
         <v>143</v>
@@ -26943,7 +26945,7 @@
         <v>349</v>
       </c>
       <c r="G42" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H42" s="29" t="s">
         <v>143</v>
@@ -27014,7 +27016,7 @@
         <v>349</v>
       </c>
       <c r="G43" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H43" s="29" t="s">
         <v>143</v>
@@ -27085,7 +27087,7 @@
         <v>349</v>
       </c>
       <c r="G44" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H44" s="29" t="s">
         <v>143</v>
@@ -27156,7 +27158,7 @@
         <v>349</v>
       </c>
       <c r="G45" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H45" s="37" t="s">
         <v>143</v>
@@ -27227,7 +27229,7 @@
         <v>349</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H46" s="29" t="s">
         <v>143</v>
@@ -27298,7 +27300,7 @@
         <v>349</v>
       </c>
       <c r="G47" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H47" s="29" t="s">
         <v>143</v>
@@ -27369,7 +27371,7 @@
         <v>349</v>
       </c>
       <c r="G48" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H48" s="29" t="s">
         <v>143</v>
@@ -27440,7 +27442,7 @@
         <v>349</v>
       </c>
       <c r="G49" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H49" s="37" t="s">
         <v>143</v>
@@ -27511,7 +27513,7 @@
         <v>349</v>
       </c>
       <c r="G50" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H50" s="29" t="s">
         <v>143</v>
@@ -27582,7 +27584,7 @@
         <v>349</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H51" s="29" t="s">
         <v>143</v>
@@ -27653,7 +27655,7 @@
         <v>349</v>
       </c>
       <c r="G52" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H52" s="29" t="s">
         <v>143</v>
@@ -27724,7 +27726,7 @@
         <v>349</v>
       </c>
       <c r="G53" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H53" s="37" t="s">
         <v>143</v>
@@ -27795,7 +27797,7 @@
         <v>349</v>
       </c>
       <c r="G54" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H54" s="29" t="s">
         <v>143</v>
@@ -27866,7 +27868,7 @@
         <v>349</v>
       </c>
       <c r="G55" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H55" s="29" t="s">
         <v>143</v>
@@ -27937,7 +27939,7 @@
         <v>349</v>
       </c>
       <c r="G56" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H56" s="29" t="s">
         <v>143</v>
@@ -28008,7 +28010,7 @@
         <v>349</v>
       </c>
       <c r="G57" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H57" s="37" t="s">
         <v>143</v>
@@ -28079,7 +28081,7 @@
         <v>349</v>
       </c>
       <c r="G58" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H58" s="29" t="s">
         <v>143</v>
@@ -28150,7 +28152,7 @@
         <v>349</v>
       </c>
       <c r="G59" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H59" s="29" t="s">
         <v>143</v>
@@ -28221,7 +28223,7 @@
         <v>349</v>
       </c>
       <c r="G60" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H60" s="29" t="s">
         <v>143</v>
@@ -28292,7 +28294,7 @@
         <v>349</v>
       </c>
       <c r="G61" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H61" s="37" t="s">
         <v>143</v>
@@ -28363,7 +28365,7 @@
         <v>349</v>
       </c>
       <c r="G62" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H62" s="29" t="s">
         <v>143</v>
@@ -28434,7 +28436,7 @@
         <v>349</v>
       </c>
       <c r="G63" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H63" s="29" t="s">
         <v>143</v>
@@ -28505,7 +28507,7 @@
         <v>349</v>
       </c>
       <c r="G64" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H64" s="29" t="s">
         <v>143</v>
@@ -28576,7 +28578,7 @@
         <v>349</v>
       </c>
       <c r="G65" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H65" s="37" t="s">
         <v>143</v>
@@ -28647,7 +28649,7 @@
         <v>349</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H66" s="29" t="s">
         <v>143</v>
@@ -28718,7 +28720,7 @@
         <v>349</v>
       </c>
       <c r="G67" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H67" s="29" t="s">
         <v>143</v>
@@ -28789,7 +28791,7 @@
         <v>349</v>
       </c>
       <c r="G68" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>143</v>
@@ -28860,7 +28862,7 @@
         <v>349</v>
       </c>
       <c r="G69" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H69" s="37" t="s">
         <v>143</v>
@@ -28931,7 +28933,7 @@
         <v>349</v>
       </c>
       <c r="G70" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H70" s="29" t="s">
         <v>143</v>
@@ -29002,7 +29004,7 @@
         <v>349</v>
       </c>
       <c r="G71" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H71" s="29" t="s">
         <v>143</v>
@@ -29073,7 +29075,7 @@
         <v>349</v>
       </c>
       <c r="G72" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H72" s="29" t="s">
         <v>143</v>
@@ -29144,7 +29146,7 @@
         <v>349</v>
       </c>
       <c r="G73" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H73" s="37" t="s">
         <v>143</v>
@@ -29215,7 +29217,7 @@
         <v>349</v>
       </c>
       <c r="G74" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H74" s="29" t="s">
         <v>143</v>
@@ -29286,7 +29288,7 @@
         <v>349</v>
       </c>
       <c r="G75" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H75" s="29" t="s">
         <v>143</v>
@@ -29357,7 +29359,7 @@
         <v>349</v>
       </c>
       <c r="G76" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>143</v>
@@ -29428,7 +29430,7 @@
         <v>349</v>
       </c>
       <c r="G77" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H77" s="37" t="s">
         <v>143</v>
@@ -29499,7 +29501,7 @@
         <v>349</v>
       </c>
       <c r="G78" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H78" s="29" t="s">
         <v>143</v>
@@ -29570,7 +29572,7 @@
         <v>349</v>
       </c>
       <c r="G79" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H79" s="29" t="s">
         <v>143</v>
@@ -29641,7 +29643,7 @@
         <v>349</v>
       </c>
       <c r="G80" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H80" s="29" t="s">
         <v>143</v>
@@ -29712,7 +29714,7 @@
         <v>349</v>
       </c>
       <c r="G81" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H81" s="37" t="s">
         <v>143</v>
@@ -29783,7 +29785,7 @@
         <v>349</v>
       </c>
       <c r="G82" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H82" s="29" t="s">
         <v>143</v>
@@ -29854,7 +29856,7 @@
         <v>349</v>
       </c>
       <c r="G83" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H83" s="29" t="s">
         <v>143</v>
@@ -29925,7 +29927,7 @@
         <v>349</v>
       </c>
       <c r="G84" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H84" s="29" t="s">
         <v>143</v>
@@ -29996,7 +29998,7 @@
         <v>349</v>
       </c>
       <c r="G85" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H85" s="37" t="s">
         <v>143</v>
@@ -30067,7 +30069,7 @@
         <v>349</v>
       </c>
       <c r="G86" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H86" s="29" t="s">
         <v>143</v>
@@ -30138,7 +30140,7 @@
         <v>349</v>
       </c>
       <c r="G87" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H87" s="29" t="s">
         <v>143</v>
@@ -30209,7 +30211,7 @@
         <v>349</v>
       </c>
       <c r="G88" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H88" s="29" t="s">
         <v>143</v>
@@ -30280,10 +30282,10 @@
         <v>349</v>
       </c>
       <c r="G89" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H89" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I89" s="38">
         <v>0.05</v>
@@ -30351,10 +30353,10 @@
         <v>349</v>
       </c>
       <c r="G90" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H90" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I90" s="30">
         <v>0.05</v>
@@ -30422,10 +30424,10 @@
         <v>349</v>
       </c>
       <c r="G91" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H91" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I91" s="30">
         <v>0.05</v>
@@ -30493,10 +30495,10 @@
         <v>349</v>
       </c>
       <c r="G92" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H92" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I92" s="30">
         <v>0.05</v>
@@ -30564,10 +30566,10 @@
         <v>349</v>
       </c>
       <c r="G93" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H93" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I93" s="38">
         <v>0.05</v>
@@ -30635,10 +30637,10 @@
         <v>349</v>
       </c>
       <c r="G94" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H94" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I94" s="30">
         <v>0.05</v>
@@ -30706,10 +30708,10 @@
         <v>349</v>
       </c>
       <c r="G95" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H95" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I95" s="30">
         <v>0.05</v>
@@ -30777,10 +30779,10 @@
         <v>349</v>
       </c>
       <c r="G96" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H96" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I96" s="30">
         <v>0.04</v>
@@ -30848,10 +30850,10 @@
         <v>349</v>
       </c>
       <c r="G97" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H97" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I97" s="38">
         <v>0.04</v>
@@ -30919,10 +30921,10 @@
         <v>349</v>
       </c>
       <c r="G98" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H98" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I98" s="30">
         <v>0.04</v>
@@ -30990,10 +30992,10 @@
         <v>349</v>
       </c>
       <c r="G99" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H99" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I99" s="30">
         <v>0.04</v>
@@ -31061,10 +31063,10 @@
         <v>349</v>
       </c>
       <c r="G100" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H100" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I100" s="30">
         <v>0.04</v>
@@ -31132,10 +31134,10 @@
         <v>349</v>
       </c>
       <c r="G101" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H101" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I101" s="38">
         <v>3.5000000000000003E-2</v>
@@ -31203,10 +31205,10 @@
         <v>349</v>
       </c>
       <c r="G102" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H102" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I102" s="30">
         <v>3.5000000000000003E-2</v>
@@ -31274,10 +31276,10 @@
         <v>349</v>
       </c>
       <c r="G103" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H103" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I103" s="30">
         <v>3.5000000000000003E-2</v>
@@ -31345,10 +31347,10 @@
         <v>349</v>
       </c>
       <c r="G104" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H104" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I104" s="30">
         <v>3.5000000000000003E-2</v>
@@ -31416,10 +31418,10 @@
         <v>349</v>
       </c>
       <c r="G105" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H105" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I105" s="38">
         <v>0.03</v>
@@ -31487,10 +31489,10 @@
         <v>349</v>
       </c>
       <c r="G106" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H106" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I106" s="30">
         <v>0.03</v>
@@ -31558,10 +31560,10 @@
         <v>349</v>
       </c>
       <c r="G107" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H107" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I107" s="30">
         <v>0.03</v>
@@ -31629,10 +31631,10 @@
         <v>349</v>
       </c>
       <c r="G108" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H108" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I108" s="30">
         <v>0.03</v>
@@ -31700,10 +31702,10 @@
         <v>349</v>
       </c>
       <c r="G109" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H109" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I109" s="38">
         <v>2.5000000000000001E-2</v>
@@ -31771,10 +31773,10 @@
         <v>349</v>
       </c>
       <c r="G110" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H110" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I110" s="30">
         <v>2.5000000000000001E-2</v>
@@ -31842,10 +31844,10 @@
         <v>349</v>
       </c>
       <c r="G111" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H111" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I111" s="30">
         <v>2.5000000000000001E-2</v>
@@ -31913,10 +31915,10 @@
         <v>349</v>
       </c>
       <c r="G112" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H112" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I112" s="30">
         <v>2.5000000000000001E-2</v>
@@ -31984,10 +31986,10 @@
         <v>349</v>
       </c>
       <c r="G113" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H113" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I113" s="38">
         <v>0.02</v>
@@ -32055,10 +32057,10 @@
         <v>349</v>
       </c>
       <c r="G114" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H114" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I114" s="30">
         <v>0.02</v>
@@ -32126,7 +32128,7 @@
         <v>349</v>
       </c>
       <c r="G115" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H115" s="29" t="s">
         <v>143</v>
@@ -32197,7 +32199,7 @@
         <v>349</v>
       </c>
       <c r="G116" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H116" s="29" t="s">
         <v>143</v>
@@ -32268,7 +32270,7 @@
         <v>349</v>
       </c>
       <c r="G117" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H117" s="29" t="s">
         <v>143</v>
@@ -32339,7 +32341,7 @@
         <v>349</v>
       </c>
       <c r="G118" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H118" s="37" t="s">
         <v>143</v>
@@ -32410,7 +32412,7 @@
         <v>349</v>
       </c>
       <c r="G119" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H119" s="29" t="s">
         <v>143</v>
@@ -32481,7 +32483,7 @@
         <v>349</v>
       </c>
       <c r="G120" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H120" s="29" t="s">
         <v>143</v>
@@ -32552,7 +32554,7 @@
         <v>349</v>
       </c>
       <c r="G121" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H121" s="29" t="s">
         <v>143</v>
@@ -32623,7 +32625,7 @@
         <v>349</v>
       </c>
       <c r="G122" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H122" s="37" t="s">
         <v>143</v>
@@ -32694,7 +32696,7 @@
         <v>349</v>
       </c>
       <c r="G123" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H123" s="29" t="s">
         <v>143</v>
@@ -32765,7 +32767,7 @@
         <v>349</v>
       </c>
       <c r="G124" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H124" s="29" t="s">
         <v>143</v>
@@ -32836,7 +32838,7 @@
         <v>349</v>
       </c>
       <c r="G125" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H125" s="29" t="s">
         <v>143</v>
@@ -32907,7 +32909,7 @@
         <v>349</v>
       </c>
       <c r="G126" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H126" s="29" t="s">
         <v>143</v>
@@ -32978,7 +32980,7 @@
         <v>349</v>
       </c>
       <c r="G127" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H127" s="37" t="s">
         <v>143</v>
@@ -33049,7 +33051,7 @@
         <v>349</v>
       </c>
       <c r="G128" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H128" s="29" t="s">
         <v>143</v>
@@ -33120,7 +33122,7 @@
         <v>349</v>
       </c>
       <c r="G129" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H129" s="29" t="s">
         <v>143</v>
@@ -33191,7 +33193,7 @@
         <v>349</v>
       </c>
       <c r="G130" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H130" s="29" t="s">
         <v>143</v>
@@ -33262,7 +33264,7 @@
         <v>349</v>
       </c>
       <c r="G131" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H131" s="37" t="s">
         <v>143</v>
@@ -33333,7 +33335,7 @@
         <v>349</v>
       </c>
       <c r="G132" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H132" s="29" t="s">
         <v>143</v>
@@ -33404,7 +33406,7 @@
         <v>349</v>
       </c>
       <c r="G133" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H133" s="29" t="s">
         <v>143</v>
@@ -33475,7 +33477,7 @@
         <v>349</v>
       </c>
       <c r="G134" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H134" s="29" t="s">
         <v>143</v>
@@ -33546,7 +33548,7 @@
         <v>349</v>
       </c>
       <c r="G135" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H135" s="29" t="s">
         <v>143</v>
@@ -33617,7 +33619,7 @@
         <v>349</v>
       </c>
       <c r="G136" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H136" s="37" t="s">
         <v>143</v>
@@ -33688,7 +33690,7 @@
         <v>349</v>
       </c>
       <c r="G137" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H137" s="29" t="s">
         <v>143</v>
@@ -33759,7 +33761,7 @@
         <v>349</v>
       </c>
       <c r="G138" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H138" s="29" t="s">
         <v>143</v>
@@ -33830,7 +33832,7 @@
         <v>349</v>
       </c>
       <c r="G139" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H139" s="29" t="s">
         <v>143</v>
@@ -33901,7 +33903,7 @@
         <v>349</v>
       </c>
       <c r="G140" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H140" s="37" t="s">
         <v>143</v>
@@ -33972,7 +33974,7 @@
         <v>349</v>
       </c>
       <c r="G141" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H141" s="29" t="s">
         <v>143</v>
@@ -34043,7 +34045,7 @@
         <v>349</v>
       </c>
       <c r="G142" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H142" s="29" t="s">
         <v>143</v>
@@ -34114,7 +34116,7 @@
         <v>349</v>
       </c>
       <c r="G143" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H143" s="29" t="s">
         <v>143</v>
@@ -34185,7 +34187,7 @@
         <v>349</v>
       </c>
       <c r="G144" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H144" s="29" t="s">
         <v>143</v>
@@ -34256,7 +34258,7 @@
         <v>349</v>
       </c>
       <c r="G145" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H145" s="37" t="s">
         <v>143</v>
@@ -34327,7 +34329,7 @@
         <v>349</v>
       </c>
       <c r="G146" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H146" s="29" t="s">
         <v>143</v>
@@ -34398,7 +34400,7 @@
         <v>349</v>
       </c>
       <c r="G147" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H147" s="29" t="s">
         <v>143</v>
@@ -34469,7 +34471,7 @@
         <v>349</v>
       </c>
       <c r="G148" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H148" s="29" t="s">
         <v>143</v>
@@ -34540,7 +34542,7 @@
         <v>349</v>
       </c>
       <c r="G149" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H149" s="37" t="s">
         <v>143</v>
@@ -34611,7 +34613,7 @@
         <v>349</v>
       </c>
       <c r="G150" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H150" s="29" t="s">
         <v>143</v>
@@ -34682,7 +34684,7 @@
         <v>349</v>
       </c>
       <c r="G151" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H151" s="29" t="s">
         <v>143</v>
@@ -34753,7 +34755,7 @@
         <v>349</v>
       </c>
       <c r="G152" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H152" s="29" t="s">
         <v>143</v>
@@ -34824,7 +34826,7 @@
         <v>349</v>
       </c>
       <c r="G153" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H153" s="29" t="s">
         <v>143</v>
@@ -34895,7 +34897,7 @@
         <v>349</v>
       </c>
       <c r="G154" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H154" s="37" t="s">
         <v>143</v>
@@ -34966,7 +34968,7 @@
         <v>349</v>
       </c>
       <c r="G155" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H155" s="29" t="s">
         <v>143</v>
@@ -35037,7 +35039,7 @@
         <v>349</v>
       </c>
       <c r="G156" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H156" s="29" t="s">
         <v>143</v>
@@ -35108,7 +35110,7 @@
         <v>349</v>
       </c>
       <c r="G157" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H157" s="29" t="s">
         <v>143</v>
@@ -35179,7 +35181,7 @@
         <v>349</v>
       </c>
       <c r="G158" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H158" s="37" t="s">
         <v>143</v>
@@ -35250,7 +35252,7 @@
         <v>349</v>
       </c>
       <c r="G159" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H159" s="29" t="s">
         <v>143</v>
@@ -35321,7 +35323,7 @@
         <v>349</v>
       </c>
       <c r="G160" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H160" s="29" t="s">
         <v>143</v>
@@ -35392,7 +35394,7 @@
         <v>349</v>
       </c>
       <c r="G161" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H161" s="29" t="s">
         <v>143</v>
@@ -35463,7 +35465,7 @@
         <v>349</v>
       </c>
       <c r="G162" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H162" s="29" t="s">
         <v>143</v>
@@ -35534,7 +35536,7 @@
         <v>349</v>
       </c>
       <c r="G163" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H163" s="37" t="s">
         <v>143</v>
@@ -35605,7 +35607,7 @@
         <v>349</v>
       </c>
       <c r="G164" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H164" s="29" t="s">
         <v>143</v>
@@ -35676,7 +35678,7 @@
         <v>349</v>
       </c>
       <c r="G165" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H165" s="29" t="s">
         <v>143</v>
@@ -35747,7 +35749,7 @@
         <v>349</v>
       </c>
       <c r="G166" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H166" s="29" t="s">
         <v>143</v>
@@ -35818,7 +35820,7 @@
         <v>349</v>
       </c>
       <c r="G167" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H167" s="37" t="s">
         <v>143</v>
@@ -35889,7 +35891,7 @@
         <v>349</v>
       </c>
       <c r="G168" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H168" s="29" t="s">
         <v>143</v>
@@ -35960,7 +35962,7 @@
         <v>349</v>
       </c>
       <c r="G169" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H169" s="29" t="s">
         <v>143</v>
@@ -36031,7 +36033,7 @@
         <v>349</v>
       </c>
       <c r="G170" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H170" s="29" t="s">
         <v>143</v>
@@ -36102,7 +36104,7 @@
         <v>349</v>
       </c>
       <c r="G171" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H171" s="29" t="s">
         <v>143</v>
@@ -36173,7 +36175,7 @@
         <v>349</v>
       </c>
       <c r="G172" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H172" s="37" t="s">
         <v>143</v>
@@ -36244,7 +36246,7 @@
         <v>349</v>
       </c>
       <c r="G173" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H173" s="29" t="s">
         <v>143</v>
@@ -36315,7 +36317,7 @@
         <v>349</v>
       </c>
       <c r="G174" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H174" s="29" t="s">
         <v>143</v>
@@ -36386,7 +36388,7 @@
         <v>349</v>
       </c>
       <c r="G175" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H175" s="29" t="s">
         <v>143</v>
@@ -36457,7 +36459,7 @@
         <v>349</v>
       </c>
       <c r="G176" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H176" s="37" t="s">
         <v>143</v>
@@ -36528,7 +36530,7 @@
         <v>349</v>
       </c>
       <c r="G177" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H177" s="29" t="s">
         <v>143</v>
@@ -36599,7 +36601,7 @@
         <v>349</v>
       </c>
       <c r="G178" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H178" s="29" t="s">
         <v>143</v>
@@ -36670,7 +36672,7 @@
         <v>349</v>
       </c>
       <c r="G179" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H179" s="29" t="s">
         <v>143</v>
@@ -36741,7 +36743,7 @@
         <v>349</v>
       </c>
       <c r="G180" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H180" s="29" t="s">
         <v>143</v>
@@ -36812,7 +36814,7 @@
         <v>349</v>
       </c>
       <c r="G181" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H181" s="37" t="s">
         <v>143</v>
@@ -36883,7 +36885,7 @@
         <v>349</v>
       </c>
       <c r="G182" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H182" s="29" t="s">
         <v>143</v>
@@ -36954,7 +36956,7 @@
         <v>349</v>
       </c>
       <c r="G183" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H183" s="29" t="s">
         <v>143</v>
@@ -37025,7 +37027,7 @@
         <v>349</v>
       </c>
       <c r="G184" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H184" s="29" t="s">
         <v>143</v>
@@ -37096,7 +37098,7 @@
         <v>349</v>
       </c>
       <c r="G185" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H185" s="37" t="s">
         <v>143</v>
@@ -37167,7 +37169,7 @@
         <v>349</v>
       </c>
       <c r="G186" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H186" s="29" t="s">
         <v>143</v>
@@ -37238,7 +37240,7 @@
         <v>349</v>
       </c>
       <c r="G187" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H187" s="29" t="s">
         <v>143</v>
@@ -37309,7 +37311,7 @@
         <v>349</v>
       </c>
       <c r="G188" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H188" s="29" t="s">
         <v>143</v>
@@ -37380,7 +37382,7 @@
         <v>349</v>
       </c>
       <c r="G189" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H189" s="29" t="s">
         <v>143</v>
@@ -37451,7 +37453,7 @@
         <v>349</v>
       </c>
       <c r="G190" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H190" s="37" t="s">
         <v>143</v>
@@ -37522,7 +37524,7 @@
         <v>349</v>
       </c>
       <c r="G191" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H191" s="29" t="s">
         <v>143</v>
@@ -37593,7 +37595,7 @@
         <v>349</v>
       </c>
       <c r="G192" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H192" s="29" t="s">
         <v>143</v>
@@ -37664,7 +37666,7 @@
         <v>349</v>
       </c>
       <c r="G193" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H193" s="29" t="s">
         <v>143</v>
@@ -37735,7 +37737,7 @@
         <v>349</v>
       </c>
       <c r="G194" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H194" s="37" t="s">
         <v>143</v>
@@ -37806,7 +37808,7 @@
         <v>349</v>
       </c>
       <c r="G195" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H195" s="29" t="s">
         <v>143</v>
@@ -37877,7 +37879,7 @@
         <v>349</v>
       </c>
       <c r="G196" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H196" s="29" t="s">
         <v>143</v>
@@ -37948,7 +37950,7 @@
         <v>349</v>
       </c>
       <c r="G197" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H197" s="29" t="s">
         <v>143</v>
@@ -38019,7 +38021,7 @@
         <v>349</v>
       </c>
       <c r="G198" s="29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H198" s="29" t="s">
         <v>143</v>
@@ -38090,7 +38092,7 @@
         <v>349</v>
       </c>
       <c r="G199" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H199" s="37" t="s">
         <v>143</v>
@@ -38161,10 +38163,10 @@
         <v>349</v>
       </c>
       <c r="G200" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H200" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I200" s="30">
         <v>7.4999999999999997E-2</v>
@@ -38232,10 +38234,10 @@
         <v>349</v>
       </c>
       <c r="G201" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H201" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I201" s="30">
         <v>7.4999999999999997E-2</v>
@@ -38303,10 +38305,10 @@
         <v>349</v>
       </c>
       <c r="G202" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H202" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I202" s="30">
         <v>7.4999999999999997E-2</v>
@@ -38374,10 +38376,10 @@
         <v>349</v>
       </c>
       <c r="G203" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H203" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I203" s="38">
         <v>6.5000000000000002E-2</v>
@@ -38445,10 +38447,10 @@
         <v>349</v>
       </c>
       <c r="G204" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H204" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I204" s="30">
         <v>6.5000000000000002E-2</v>
@@ -38516,10 +38518,10 @@
         <v>349</v>
       </c>
       <c r="G205" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H205" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I205" s="30">
         <v>6.5000000000000002E-2</v>
@@ -38587,10 +38589,10 @@
         <v>349</v>
       </c>
       <c r="G206" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H206" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I206" s="30">
         <v>6.5000000000000002E-2</v>
@@ -38658,10 +38660,10 @@
         <v>349</v>
       </c>
       <c r="G207" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H207" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I207" s="30">
         <v>0.05</v>
@@ -38729,10 +38731,10 @@
         <v>349</v>
       </c>
       <c r="G208" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H208" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I208" s="38">
         <v>0.05</v>
@@ -38800,10 +38802,10 @@
         <v>349</v>
       </c>
       <c r="G209" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H209" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I209" s="30">
         <v>0.05</v>
@@ -38871,10 +38873,10 @@
         <v>349</v>
       </c>
       <c r="G210" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H210" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I210" s="30">
         <v>0.05</v>
@@ -38942,10 +38944,10 @@
         <v>349</v>
       </c>
       <c r="G211" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H211" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I211" s="30">
         <v>0.05</v>
@@ -39013,10 +39015,10 @@
         <v>349</v>
       </c>
       <c r="G212" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H212" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I212" s="38">
         <v>0.05</v>
@@ -39084,10 +39086,10 @@
         <v>349</v>
       </c>
       <c r="G213" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H213" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I213" s="30">
         <v>0.05</v>
@@ -39155,10 +39157,10 @@
         <v>349</v>
       </c>
       <c r="G214" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H214" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I214" s="30">
         <v>0.05</v>
@@ -39218,8 +39220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50DD9B1-E32D-4618-AC3A-A0F8971F8A87}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39252,7 +39254,7 @@
         <v>121</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>518</v>
+        <v>158</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>122</v>
@@ -39273,13 +39275,13 @@
         <v>123</v>
       </c>
       <c r="L1" s="26" t="s">
+        <v>518</v>
+      </c>
+      <c r="M1" s="26" t="s">
         <v>519</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>520</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>521</v>
       </c>
       <c r="O1" s="26" t="s">
         <v>442</v>
@@ -39311,7 +39313,7 @@
         <v>517</v>
       </c>
       <c r="G2" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H2" s="47" t="s">
         <v>441</v>
@@ -39364,7 +39366,7 @@
         <v>517</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H3" s="47" t="s">
         <v>441</v>
@@ -39417,7 +39419,7 @@
         <v>517</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H4" s="47" t="s">
         <v>441</v>
@@ -39470,7 +39472,7 @@
         <v>517</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H5" s="47" t="s">
         <v>441</v>
@@ -39523,7 +39525,7 @@
         <v>517</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H6" s="47" t="s">
         <v>441</v>
@@ -39576,7 +39578,7 @@
         <v>517</v>
       </c>
       <c r="G7" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H7" s="47" t="s">
         <v>441</v>
@@ -39629,7 +39631,7 @@
         <v>517</v>
       </c>
       <c r="G8" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H8" s="47" t="s">
         <v>441</v>
@@ -39682,7 +39684,7 @@
         <v>517</v>
       </c>
       <c r="G9" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H9" s="47" t="s">
         <v>441</v>
@@ -39735,7 +39737,7 @@
         <v>517</v>
       </c>
       <c r="G10" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H10" s="47" t="s">
         <v>441</v>
@@ -39788,7 +39790,7 @@
         <v>517</v>
       </c>
       <c r="G11" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H11" s="47" t="s">
         <v>441</v>
@@ -39841,7 +39843,7 @@
         <v>517</v>
       </c>
       <c r="G12" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H12" s="47" t="s">
         <v>441</v>
@@ -39894,7 +39896,7 @@
         <v>517</v>
       </c>
       <c r="G13" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H13" s="47" t="s">
         <v>441</v>
@@ -39947,7 +39949,7 @@
         <v>517</v>
       </c>
       <c r="G14" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H14" s="47" t="s">
         <v>441</v>
@@ -40000,7 +40002,7 @@
         <v>517</v>
       </c>
       <c r="G15" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H15" s="47" t="s">
         <v>441</v>
@@ -40053,7 +40055,7 @@
         <v>517</v>
       </c>
       <c r="G16" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H16" s="47" t="s">
         <v>441</v>
@@ -40106,7 +40108,7 @@
         <v>517</v>
       </c>
       <c r="G17" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H17" s="47" t="s">
         <v>441</v>
@@ -40159,7 +40161,7 @@
         <v>517</v>
       </c>
       <c r="G18" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H18" s="47" t="s">
         <v>441</v>
@@ -40212,7 +40214,7 @@
         <v>517</v>
       </c>
       <c r="G19" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H19" s="47" t="s">
         <v>441</v>
@@ -40265,7 +40267,7 @@
         <v>517</v>
       </c>
       <c r="G20" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H20" s="47" t="s">
         <v>441</v>
@@ -40318,7 +40320,7 @@
         <v>517</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H21" s="47" t="s">
         <v>441</v>
@@ -40371,7 +40373,7 @@
         <v>517</v>
       </c>
       <c r="G22" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H22" s="47" t="s">
         <v>441</v>
@@ -40424,7 +40426,7 @@
         <v>517</v>
       </c>
       <c r="G23" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H23" s="47" t="s">
         <v>441</v>
@@ -40477,7 +40479,7 @@
         <v>517</v>
       </c>
       <c r="G24" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H24" s="47" t="s">
         <v>441</v>
@@ -40530,7 +40532,7 @@
         <v>517</v>
       </c>
       <c r="G25" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H25" s="47" t="s">
         <v>441</v>
@@ -40583,7 +40585,7 @@
         <v>517</v>
       </c>
       <c r="G26" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H26" s="47" t="s">
         <v>441</v>
@@ -40636,7 +40638,7 @@
         <v>517</v>
       </c>
       <c r="G27" s="47" t="s">
-        <v>146</v>
+        <v>524</v>
       </c>
       <c r="H27" s="47" t="s">
         <v>441</v>
@@ -40689,7 +40691,7 @@
         <v>517</v>
       </c>
       <c r="G28" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H28" s="47" t="s">
         <v>441</v>
@@ -40742,7 +40744,7 @@
         <v>517</v>
       </c>
       <c r="G29" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H29" s="47" t="s">
         <v>441</v>
@@ -40795,7 +40797,7 @@
         <v>517</v>
       </c>
       <c r="G30" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H30" s="47" t="s">
         <v>441</v>
@@ -40848,7 +40850,7 @@
         <v>517</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H31" s="47" t="s">
         <v>441</v>
@@ -40901,7 +40903,7 @@
         <v>517</v>
       </c>
       <c r="G32" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H32" s="47" t="s">
         <v>441</v>
@@ -40954,7 +40956,7 @@
         <v>517</v>
       </c>
       <c r="G33" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H33" s="47" t="s">
         <v>441</v>
@@ -41007,7 +41009,7 @@
         <v>517</v>
       </c>
       <c r="G34" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H34" s="47" t="s">
         <v>441</v>
@@ -41060,7 +41062,7 @@
         <v>517</v>
       </c>
       <c r="G35" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H35" s="47" t="s">
         <v>441</v>
@@ -41113,7 +41115,7 @@
         <v>517</v>
       </c>
       <c r="G36" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H36" s="47" t="s">
         <v>441</v>
@@ -41166,7 +41168,7 @@
         <v>517</v>
       </c>
       <c r="G37" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H37" s="47" t="s">
         <v>441</v>
@@ -41219,7 +41221,7 @@
         <v>517</v>
       </c>
       <c r="G38" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H38" s="47" t="s">
         <v>441</v>
@@ -41272,7 +41274,7 @@
         <v>517</v>
       </c>
       <c r="G39" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H39" s="47" t="s">
         <v>441</v>
@@ -41325,7 +41327,7 @@
         <v>517</v>
       </c>
       <c r="G40" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H40" s="47" t="s">
         <v>441</v>
@@ -41378,7 +41380,7 @@
         <v>517</v>
       </c>
       <c r="G41" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H41" s="47" t="s">
         <v>441</v>
@@ -41431,7 +41433,7 @@
         <v>517</v>
       </c>
       <c r="G42" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H42" s="47" t="s">
         <v>441</v>
@@ -41484,7 +41486,7 @@
         <v>517</v>
       </c>
       <c r="G43" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H43" s="47" t="s">
         <v>441</v>
@@ -41537,7 +41539,7 @@
         <v>517</v>
       </c>
       <c r="G44" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H44" s="47" t="s">
         <v>441</v>
@@ -41590,7 +41592,7 @@
         <v>517</v>
       </c>
       <c r="G45" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H45" s="47" t="s">
         <v>441</v>
@@ -41643,7 +41645,7 @@
         <v>517</v>
       </c>
       <c r="G46" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H46" s="47" t="s">
         <v>441</v>
@@ -41696,7 +41698,7 @@
         <v>517</v>
       </c>
       <c r="G47" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H47" s="47" t="s">
         <v>441</v>
@@ -41749,7 +41751,7 @@
         <v>517</v>
       </c>
       <c r="G48" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H48" s="47" t="s">
         <v>441</v>
@@ -41802,7 +41804,7 @@
         <v>517</v>
       </c>
       <c r="G49" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H49" s="47" t="s">
         <v>441</v>
@@ -41855,7 +41857,7 @@
         <v>517</v>
       </c>
       <c r="G50" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H50" s="47" t="s">
         <v>441</v>
@@ -41908,7 +41910,7 @@
         <v>517</v>
       </c>
       <c r="G51" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H51" s="47" t="s">
         <v>441</v>
@@ -41961,7 +41963,7 @@
         <v>517</v>
       </c>
       <c r="G52" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H52" s="47" t="s">
         <v>441</v>
@@ -42014,7 +42016,7 @@
         <v>517</v>
       </c>
       <c r="G53" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H53" s="47" t="s">
         <v>441</v>
@@ -42067,7 +42069,7 @@
         <v>517</v>
       </c>
       <c r="G54" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H54" s="47" t="s">
         <v>441</v>
@@ -42120,7 +42122,7 @@
         <v>517</v>
       </c>
       <c r="G55" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H55" s="47" t="s">
         <v>441</v>
@@ -42173,7 +42175,7 @@
         <v>517</v>
       </c>
       <c r="G56" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H56" s="47" t="s">
         <v>441</v>
@@ -42226,7 +42228,7 @@
         <v>517</v>
       </c>
       <c r="G57" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H57" s="47" t="s">
         <v>441</v>
@@ -42279,7 +42281,7 @@
         <v>517</v>
       </c>
       <c r="G58" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H58" s="47" t="s">
         <v>441</v>
@@ -42332,7 +42334,7 @@
         <v>517</v>
       </c>
       <c r="G59" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H59" s="47" t="s">
         <v>441</v>
@@ -42385,7 +42387,7 @@
         <v>517</v>
       </c>
       <c r="G60" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H60" s="47" t="s">
         <v>441</v>
@@ -42438,7 +42440,7 @@
         <v>517</v>
       </c>
       <c r="G61" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H61" s="47" t="s">
         <v>441</v>
@@ -42491,7 +42493,7 @@
         <v>517</v>
       </c>
       <c r="G62" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H62" s="47" t="s">
         <v>441</v>
@@ -42544,7 +42546,7 @@
         <v>517</v>
       </c>
       <c r="G63" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H63" s="47" t="s">
         <v>441</v>
@@ -42597,7 +42599,7 @@
         <v>517</v>
       </c>
       <c r="G64" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H64" s="47" t="s">
         <v>441</v>
@@ -42650,7 +42652,7 @@
         <v>517</v>
       </c>
       <c r="G65" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H65" s="47" t="s">
         <v>441</v>
@@ -42703,7 +42705,7 @@
         <v>517</v>
       </c>
       <c r="G66" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H66" s="47" t="s">
         <v>441</v>
@@ -42756,7 +42758,7 @@
         <v>517</v>
       </c>
       <c r="G67" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H67" s="47" t="s">
         <v>441</v>
@@ -42809,7 +42811,7 @@
         <v>517</v>
       </c>
       <c r="G68" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H68" s="47" t="s">
         <v>441</v>
@@ -42862,7 +42864,7 @@
         <v>517</v>
       </c>
       <c r="G69" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H69" s="47" t="s">
         <v>441</v>
@@ -42915,7 +42917,7 @@
         <v>517</v>
       </c>
       <c r="G70" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H70" s="47" t="s">
         <v>441</v>
@@ -42968,7 +42970,7 @@
         <v>517</v>
       </c>
       <c r="G71" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H71" s="47" t="s">
         <v>441</v>
@@ -43021,7 +43023,7 @@
         <v>517</v>
       </c>
       <c r="G72" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H72" s="47" t="s">
         <v>441</v>
@@ -43074,7 +43076,7 @@
         <v>517</v>
       </c>
       <c r="G73" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H73" s="47" t="s">
         <v>441</v>
@@ -43127,7 +43129,7 @@
         <v>517</v>
       </c>
       <c r="G74" s="47" t="s">
-        <v>147</v>
+        <v>523</v>
       </c>
       <c r="H74" s="47" t="s">
         <v>441</v>

</xml_diff>